<commit_message>
Bug correction in the add_patterns function
</commit_message>
<xml_diff>
--- a/Results_CG.xlsx
+++ b/Results_CG.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F6B903CE-A966-4B37-9B65-FF7D8DB6156E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BBD42BB9-9E92-46AE-9698-195C9FE14B27}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
   <si>
     <t>Instance name</t>
   </si>
@@ -162,6 +162,12 @@
   <si>
     <t>Improvement/ILP</t>
   </si>
+  <si>
+    <t>Optimal</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
 </sst>
 </file>
 
@@ -212,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,6 +233,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -352,7 +361,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$T$27:$T$51</c:f>
+              <c:f>Sheet1!$U$27:$U$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -436,7 +445,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$U$27:$U$51</c:f>
+              <c:f>Sheet1!$V$27:$V$51</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="25"/>
@@ -555,7 +564,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$T$27:$T$51</c:f>
+              <c:f>Sheet1!$U$27:$U$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -639,7 +648,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$V$27:$V$51</c:f>
+              <c:f>Sheet1!$W$27:$W$51</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1170,7 +1179,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$T$60:$T$84</c:f>
+              <c:f>Sheet1!$U$60:$U$84</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1254,7 +1263,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$U$60:$U$84</c:f>
+              <c:f>Sheet1!$V$60:$V$84</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1373,7 +1382,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$T$60:$T$84</c:f>
+              <c:f>Sheet1!$U$60:$U$84</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1457,7 +1466,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$V$60:$V$84</c:f>
+              <c:f>Sheet1!$W$60:$W$84</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1994,7 +2003,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$X$27:$X$50</c:f>
+              <c:f>Sheet1!$Y$27:$Y$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -2075,7 +2084,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Y$27:$Y$50</c:f>
+              <c:f>Sheet1!$Z$27:$Z$50</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="24"/>
@@ -2191,7 +2200,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$X$27:$X$50</c:f>
+              <c:f>Sheet1!$Y$27:$Y$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -2272,7 +2281,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Z$27:$Z$50</c:f>
+              <c:f>Sheet1!$AA$27:$AA$50</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="24"/>
@@ -4410,7 +4419,7 @@
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>933450</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -4740,10 +4749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:Z84"/>
+  <dimension ref="C3:AA84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="I80" sqref="I80"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4756,36 +4765,36 @@
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="12" width="11.140625" customWidth="1"/>
-    <col min="14" max="15" width="19.7109375" customWidth="1"/>
-    <col min="16" max="17" width="17.28515625" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" customWidth="1"/>
-    <col min="21" max="21" width="12.85546875" customWidth="1"/>
-    <col min="23" max="23" width="34.140625" customWidth="1"/>
+    <col min="11" max="13" width="11.140625" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" customWidth="1"/>
+    <col min="17" max="18" width="17.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" customWidth="1"/>
+    <col min="22" max="22" width="12.85546875" customWidth="1"/>
+    <col min="24" max="24" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="S3" t="s">
+    <row r="3" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="T3" t="s">
         <v>15</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="N4" s="4" t="s">
+    <row r="4" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="O4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="4"/>
-      <c r="S4" t="s">
+      <c r="R4" s="6"/>
+      <c r="T4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>5</v>
@@ -4808,15 +4817,18 @@
       <c r="L5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="1"/>
-      <c r="S5" t="s">
+      <c r="M5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="T5" t="s">
         <v>42</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
@@ -4849,28 +4861,31 @@
       <c r="L6" s="1">
         <v>4001</v>
       </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="3">
+      <c r="M6" s="4">
+        <v>4037</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="3">
         <f>(L6-I6)/I6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="5">
+      <c r="P6" s="5">
         <f>L6-I6</f>
         <v>0</v>
       </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="3">
         <f>(L6-J6)/J6</f>
         <v>-8.9175130047064646E-3</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="R6" s="5">
         <f>L6-J6</f>
         <v>-36</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
@@ -4900,28 +4915,31 @@
       <c r="L7" s="2">
         <v>4073</v>
       </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="3">
+      <c r="M7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="3">
         <f>(L7-I7)/I7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="5">
-        <f t="shared" ref="O7:O10" si="0">L7-I7</f>
+      <c r="P7" s="5">
+        <f t="shared" ref="P7:P10" si="0">L7-I7</f>
         <v>0</v>
       </c>
-      <c r="P7" s="3">
-        <f t="shared" ref="P7:P31" si="1">(L7-J7)/J7</f>
+      <c r="Q7" s="3">
+        <f t="shared" ref="Q7:Q31" si="1">(L7-J7)/J7</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="5">
-        <f t="shared" ref="Q7:Q10" si="2">L7-J7</f>
+      <c r="R7" s="5">
+        <f t="shared" ref="R7:R10" si="2">L7-J7</f>
         <v>0</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
@@ -4951,25 +4969,28 @@
       <c r="L8" s="2">
         <v>4097</v>
       </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="3">
+      <c r="M8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="3">
         <f>(L8-I8)/I8</f>
         <v>1.7114914425427872E-3</v>
       </c>
-      <c r="O8" s="5">
+      <c r="P8" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="P8" s="3">
+      <c r="Q8" s="3">
         <f t="shared" si="1"/>
         <v>1.7114914425427872E-3</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="R8" s="5">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
@@ -4999,25 +5020,28 @@
       <c r="L9" s="2">
         <v>4129</v>
       </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="3">
-        <f t="shared" ref="N9:N31" si="3">(L9-I9)/I9</f>
+      <c r="M9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="3">
+        <f t="shared" ref="O9:O31" si="3">(L9-I9)/I9</f>
         <v>7.2709646146388749E-4</v>
       </c>
-      <c r="O9" s="5">
+      <c r="P9" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="P9" s="3">
+      <c r="Q9" s="3">
         <f t="shared" si="1"/>
         <v>7.2709646146388749E-4</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="R9" s="5">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
@@ -5047,25 +5071,28 @@
       <c r="L10" s="2">
         <v>4164</v>
       </c>
-      <c r="M10" s="1"/>
-      <c r="N10" s="3">
+      <c r="M10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="3">
         <f t="shared" si="3"/>
         <v>2.4021138601969732E-4</v>
       </c>
-      <c r="O10" s="5">
+      <c r="P10" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P10" s="3">
+      <c r="Q10" s="3">
         <f t="shared" si="1"/>
         <v>2.4021138601969732E-4</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="R10" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
@@ -5087,49 +5114,54 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="3" t="e">
+      <c r="M11" s="4"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="3" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O11" s="5"/>
-      <c r="P11" s="3" t="e">
+      <c r="P11" s="5"/>
+      <c r="Q11" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="N12" s="3"/>
+    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="M12" s="4"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="N13" s="3"/>
+    <row r="13" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="M13" s="4"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="T13" t="s">
+      <c r="R13" s="3"/>
+      <c r="U13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="N14" s="3"/>
+    <row r="14" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="M14" s="4"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="T14" t="s">
+      <c r="R14" s="3"/>
+      <c r="U14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="N15" s="3"/>
+    <row r="15" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="M15" s="4"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="F16" s="1" t="s">
         <v>5</v>
@@ -5148,12 +5180,13 @@
       <c r="L16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N16" s="3"/>
+      <c r="M16" s="4"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>0</v>
       </c>
@@ -5186,27 +5219,30 @@
       <c r="L17" s="2">
         <v>576</v>
       </c>
-      <c r="N17" s="3">
+      <c r="M17" s="4">
+        <v>576</v>
+      </c>
+      <c r="O17" s="3">
         <f t="shared" si="3"/>
         <v>1.9469026548672566E-2</v>
       </c>
-      <c r="O17" s="5">
+      <c r="P17" s="5">
         <f>L17-I17</f>
         <v>11</v>
       </c>
-      <c r="P17" s="3">
+      <c r="Q17" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="5">
+      <c r="R17" s="5">
         <f>L17-J17</f>
         <v>0</v>
       </c>
-      <c r="W17" t="s">
+      <c r="X17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
@@ -5236,24 +5272,27 @@
       <c r="L18" s="2">
         <v>596</v>
       </c>
-      <c r="N18" s="3">
+      <c r="M18" s="4">
+        <v>597</v>
+      </c>
+      <c r="O18" s="3">
         <f t="shared" si="3"/>
         <v>5.0590219224283303E-3</v>
       </c>
-      <c r="O18" s="5">
-        <f t="shared" ref="O18:O21" si="4">L18-I18</f>
+      <c r="P18" s="5">
+        <f t="shared" ref="P18:P21" si="4">L18-I18</f>
         <v>3</v>
       </c>
-      <c r="P18" s="3">
+      <c r="Q18" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="5">
-        <f t="shared" ref="Q18:Q21" si="5">L18-J18</f>
+      <c r="R18" s="5">
+        <f t="shared" ref="R18:R21" si="5">L18-J18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>2</v>
       </c>
@@ -5283,27 +5322,30 @@
       <c r="L19" s="2">
         <v>609</v>
       </c>
-      <c r="N19" s="3">
+      <c r="M19" s="4">
+        <v>617</v>
+      </c>
+      <c r="O19" s="3">
         <f t="shared" si="3"/>
         <v>2.1812080536912751E-2</v>
       </c>
-      <c r="O19" s="5">
+      <c r="P19" s="5">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="P19" s="3">
+      <c r="Q19" s="3">
         <f t="shared" si="1"/>
         <v>8.2781456953642391E-3</v>
       </c>
-      <c r="Q19" s="5">
+      <c r="R19" s="5">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="W19" t="s">
+      <c r="X19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
@@ -5333,27 +5375,30 @@
       <c r="L20" s="2">
         <v>620</v>
       </c>
-      <c r="N20" s="3">
+      <c r="M20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O20" s="3">
         <f t="shared" si="3"/>
         <v>1.9736842105263157E-2</v>
       </c>
-      <c r="O20" s="5">
+      <c r="P20" s="5">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="P20" s="3">
+      <c r="Q20" s="3">
         <f t="shared" si="1"/>
         <v>3.2362459546925568E-3</v>
       </c>
-      <c r="Q20" s="5">
+      <c r="R20" s="5">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
@@ -5383,27 +5428,30 @@
       <c r="L21" s="2">
         <v>643</v>
       </c>
-      <c r="N21" s="3">
+      <c r="M21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O21" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O21" s="5">
+      <c r="P21" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P21" s="3">
+      <c r="Q21" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q21" s="5">
+      <c r="R21" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W21" t="s">
+      <c r="X21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
@@ -5425,33 +5473,36 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="N22" s="3" t="e">
+      <c r="M22" s="4"/>
+      <c r="O22" s="3" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3" t="e">
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q22" s="3"/>
-      <c r="W22" t="s">
+      <c r="R22" s="3"/>
+      <c r="X22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="N23" s="3"/>
+    <row r="23" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="M23" s="4"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="N24" s="3"/>
+    <row r="24" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="M24" s="4"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
     </row>
-    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="F25" s="1" t="s">
         <v>5</v>
@@ -5470,12 +5521,13 @@
       <c r="L25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N25" s="3"/>
+      <c r="M25" s="4"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
     </row>
-    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>0</v>
       </c>
@@ -5508,24 +5560,27 @@
       <c r="L26" s="1">
         <v>2372</v>
       </c>
-      <c r="N26" s="3">
+      <c r="M26" s="4">
+        <v>2415</v>
+      </c>
+      <c r="O26" s="3">
         <f t="shared" si="3"/>
         <v>7.9162875341219296E-2</v>
       </c>
-      <c r="O26" s="5">
+      <c r="P26" s="5">
         <f>L26-I26</f>
         <v>174</v>
       </c>
-      <c r="P26" s="3">
+      <c r="Q26" s="3">
         <f t="shared" si="1"/>
         <v>-1.7805383022774329E-2</v>
       </c>
-      <c r="Q26" s="5">
+      <c r="R26" s="5">
         <f>L26-J26</f>
         <v>-43</v>
       </c>
     </row>
-    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>1</v>
       </c>
@@ -5555,42 +5610,45 @@
       <c r="L27" s="2">
         <v>2614</v>
       </c>
-      <c r="N27" s="3">
+      <c r="M27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O27" s="3">
         <f t="shared" si="3"/>
         <v>2.7111984282907661E-2</v>
       </c>
-      <c r="O27" s="5">
-        <f t="shared" ref="O27:O30" si="6">L27-I27</f>
+      <c r="P27" s="5">
+        <f t="shared" ref="P27:P30" si="6">L27-I27</f>
         <v>69</v>
       </c>
-      <c r="P27" s="3">
+      <c r="Q27" s="3">
         <f t="shared" si="1"/>
         <v>2.7111984282907661E-2</v>
       </c>
-      <c r="Q27" s="5">
-        <f t="shared" ref="Q27:Q30" si="7">L27-J27</f>
+      <c r="R27" s="5">
+        <f t="shared" ref="R27:R30" si="7">L27-J27</f>
         <v>69</v>
       </c>
-      <c r="T27" s="1">
+      <c r="U27" s="1">
         <v>768</v>
       </c>
-      <c r="U27" s="3">
+      <c r="V27" s="3">
         <v>0</v>
       </c>
-      <c r="V27" s="3">
+      <c r="W27" s="3">
         <v>1.9469026548672566E-2</v>
       </c>
-      <c r="X27" s="1">
+      <c r="Y27" s="1">
         <v>768</v>
       </c>
-      <c r="Y27" s="5">
+      <c r="Z27" s="5">
         <v>0</v>
       </c>
-      <c r="Z27" s="5">
+      <c r="AA27" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
@@ -5620,42 +5678,45 @@
       <c r="L28" s="2">
         <v>2653</v>
       </c>
-      <c r="N28" s="3">
+      <c r="M28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O28" s="3">
         <f t="shared" si="3"/>
         <v>7.9787234042553185E-3</v>
       </c>
-      <c r="O28" s="5">
+      <c r="P28" s="5">
         <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="P28" s="3">
+      <c r="Q28" s="3">
         <f t="shared" si="1"/>
         <v>7.9787234042553185E-3</v>
       </c>
-      <c r="Q28" s="5">
+      <c r="R28" s="5">
         <f t="shared" si="7"/>
         <v>21</v>
       </c>
-      <c r="T28" s="1">
+      <c r="U28" s="1">
         <v>1151</v>
       </c>
-      <c r="U28" s="3">
+      <c r="V28" s="3">
         <v>-1.8439716312056736E-2</v>
       </c>
-      <c r="V28" s="3">
+      <c r="W28" s="3">
         <v>2.3668639053254437E-2</v>
       </c>
-      <c r="X28" s="1">
+      <c r="Y28" s="1">
         <v>1151</v>
       </c>
-      <c r="Y28" s="5">
+      <c r="Z28" s="5">
         <v>-13</v>
       </c>
-      <c r="Z28" s="5">
+      <c r="AA28" s="5">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
@@ -5685,42 +5746,45 @@
       <c r="L29" s="2">
         <v>2713</v>
       </c>
-      <c r="N29" s="3">
+      <c r="M29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O29" s="3">
         <f t="shared" si="3"/>
         <v>2.216475803472479E-3</v>
       </c>
-      <c r="O29" s="5">
+      <c r="P29" s="5">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="P29" s="3">
+      <c r="Q29" s="3">
         <f t="shared" si="1"/>
         <v>2.216475803472479E-3</v>
       </c>
-      <c r="Q29" s="5">
+      <c r="R29" s="5">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="T29" s="1">
+      <c r="U29" s="1">
         <v>1536</v>
       </c>
-      <c r="U29" s="3">
+      <c r="V29" s="3">
         <v>0</v>
       </c>
-      <c r="V29" s="3">
+      <c r="W29" s="3">
         <v>5.0590219224283303E-3</v>
       </c>
-      <c r="X29" s="1">
+      <c r="Y29" s="1">
         <v>1536</v>
       </c>
-      <c r="Y29" s="5">
+      <c r="Z29" s="5">
         <v>0</v>
       </c>
-      <c r="Z29" s="5">
+      <c r="AA29" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
@@ -5750,42 +5814,45 @@
       <c r="L30" s="2">
         <v>2800</v>
       </c>
-      <c r="N30" s="3">
+      <c r="M30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O30" s="3">
         <f t="shared" si="3"/>
         <v>6.4701653486700216E-3</v>
       </c>
-      <c r="O30" s="5">
+      <c r="P30" s="5">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="P30" s="3">
+      <c r="Q30" s="3">
         <f t="shared" si="1"/>
         <v>6.4701653486700216E-3</v>
       </c>
-      <c r="Q30" s="5">
+      <c r="R30" s="5">
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="T30" s="1">
+      <c r="U30" s="1">
         <v>2302</v>
       </c>
-      <c r="U30" s="3">
+      <c r="V30" s="3">
         <v>-1.3280212483399733E-3</v>
       </c>
-      <c r="V30" s="3">
+      <c r="W30" s="3">
         <v>1.3315579227696406E-3</v>
       </c>
-      <c r="X30" s="1">
+      <c r="Y30" s="1">
         <v>2302</v>
       </c>
-      <c r="Y30" s="5">
+      <c r="Z30" s="5">
         <v>-1</v>
       </c>
-      <c r="Z30" s="5">
+      <c r="AA30" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
@@ -5807,76 +5874,79 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-      <c r="N31" s="3" t="e">
+      <c r="M31" s="4"/>
+      <c r="O31" s="3" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3" t="e">
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q31" s="3"/>
-      <c r="T31" s="1">
+      <c r="R31" s="3"/>
+      <c r="U31" s="1">
         <v>2304</v>
       </c>
-      <c r="U31" s="3">
+      <c r="V31" s="3">
         <v>8.2781456953642391E-3</v>
       </c>
-      <c r="V31" s="3">
+      <c r="W31" s="3">
         <v>2.1812080536912751E-2</v>
       </c>
-      <c r="X31" s="1">
+      <c r="Y31" s="1">
         <v>2304</v>
       </c>
-      <c r="Y31" s="5">
+      <c r="Z31" s="5">
         <v>5</v>
       </c>
-      <c r="Z31" s="5">
+      <c r="AA31" s="5">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="T32" s="1">
+    <row r="32" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="M32" s="4"/>
+      <c r="U32" s="1">
         <v>3072</v>
       </c>
-      <c r="U32" s="3">
+      <c r="V32" s="3">
         <v>3.2362459546925568E-3</v>
       </c>
-      <c r="V32" s="3">
+      <c r="W32" s="3">
         <v>1.9736842105263157E-2</v>
       </c>
-      <c r="X32" s="1">
+      <c r="Y32" s="1">
         <v>3072</v>
       </c>
-      <c r="Y32" s="5">
+      <c r="Z32" s="5">
         <v>2</v>
       </c>
-      <c r="Z32" s="5">
+      <c r="AA32" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="T33" s="1">
+    <row r="33" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="M33" s="4"/>
+      <c r="U33" s="1">
         <v>3453</v>
       </c>
-      <c r="U33" s="3">
+      <c r="V33" s="3">
         <v>7.7319587628865982E-3</v>
       </c>
-      <c r="V33" s="3">
+      <c r="W33" s="3">
         <v>1.5584415584415584E-2</v>
       </c>
-      <c r="X33" s="1">
+      <c r="Y33" s="1">
         <v>3453</v>
       </c>
-      <c r="Y33" s="5">
+      <c r="Z33" s="5">
         <v>6</v>
       </c>
-      <c r="Z33" s="5">
+      <c r="AA33" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="F34" s="1" t="s">
         <v>5</v>
@@ -5895,30 +5965,31 @@
       <c r="L34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N34" s="3"/>
+      <c r="M34" s="4"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
-      <c r="T34" s="1">
+      <c r="R34" s="3"/>
+      <c r="U34" s="1">
         <v>3840</v>
-      </c>
-      <c r="U34" s="3">
-        <v>0</v>
       </c>
       <c r="V34" s="3">
         <v>0</v>
       </c>
-      <c r="X34" s="1">
+      <c r="W34" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="1">
         <v>3840</v>
-      </c>
-      <c r="Y34" s="5">
-        <v>0</v>
       </c>
       <c r="Z34" s="5">
         <v>0</v>
       </c>
+      <c r="AA34" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>0</v>
       </c>
@@ -5951,42 +6022,45 @@
       <c r="L35" s="1">
         <v>692</v>
       </c>
-      <c r="N35" s="3">
-        <f t="shared" ref="N35:N40" si="8">(L35-I35)/I35</f>
+      <c r="M35" s="4">
+        <v>705</v>
+      </c>
+      <c r="O35" s="3">
+        <f t="shared" ref="O35:O40" si="8">(L35-I35)/I35</f>
         <v>2.3668639053254437E-2</v>
       </c>
-      <c r="O35" s="5">
+      <c r="P35" s="5">
         <f>L35-I35</f>
         <v>16</v>
       </c>
-      <c r="P35" s="3">
-        <f t="shared" ref="P35:P40" si="9">(L35-J35)/J35</f>
+      <c r="Q35" s="3">
+        <f t="shared" ref="Q35:Q40" si="9">(L35-J35)/J35</f>
         <v>-1.8439716312056736E-2</v>
       </c>
-      <c r="Q35" s="5">
+      <c r="R35" s="5">
         <f>L35-J35</f>
         <v>-13</v>
       </c>
-      <c r="T35" s="1">
+      <c r="U35" s="1">
         <v>4521</v>
       </c>
-      <c r="U35" s="3">
+      <c r="V35" s="3">
         <v>-8.9175130047064646E-3</v>
       </c>
-      <c r="V35" s="3">
+      <c r="W35" s="3">
         <v>0</v>
       </c>
-      <c r="X35" s="1">
+      <c r="Y35" s="1">
         <v>4521</v>
       </c>
-      <c r="Y35" s="5">
+      <c r="Z35" s="5">
         <v>-36</v>
       </c>
-      <c r="Z35" s="5">
+      <c r="AA35" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>1</v>
       </c>
@@ -6016,42 +6090,45 @@
       <c r="L36" s="1">
         <v>752</v>
       </c>
-      <c r="N36" s="3">
+      <c r="M36" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O36" s="3">
         <f t="shared" si="8"/>
         <v>1.3315579227696406E-3</v>
       </c>
-      <c r="O36" s="5">
-        <f t="shared" ref="O36:O39" si="10">L36-I36</f>
+      <c r="P36" s="5">
+        <f t="shared" ref="P36:P40" si="10">L36-I36</f>
         <v>1</v>
       </c>
-      <c r="P36" s="3">
+      <c r="Q36" s="3">
         <f t="shared" si="9"/>
         <v>-1.3280212483399733E-3</v>
       </c>
-      <c r="Q36" s="5">
-        <f t="shared" ref="Q36:Q39" si="11">L36-J36</f>
+      <c r="R36" s="5">
+        <f t="shared" ref="R36:R40" si="11">L36-J36</f>
         <v>-1</v>
       </c>
-      <c r="T36" s="1">
+      <c r="U36" s="1">
         <v>4604</v>
-      </c>
-      <c r="U36" s="3">
-        <v>7.4257425742574254E-3</v>
       </c>
       <c r="V36" s="3">
         <v>7.4257425742574254E-3</v>
       </c>
-      <c r="X36" s="1">
+      <c r="W36" s="3">
+        <v>7.4257425742574254E-3</v>
+      </c>
+      <c r="Y36" s="1">
         <v>4604</v>
-      </c>
-      <c r="Y36" s="5">
-        <v>6</v>
       </c>
       <c r="Z36" s="5">
         <v>6</v>
       </c>
+      <c r="AA36" s="5">
+        <v>6</v>
+      </c>
     </row>
-    <row r="37" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>2</v>
       </c>
@@ -6081,42 +6158,45 @@
       <c r="L37" s="2">
         <v>782</v>
       </c>
-      <c r="N37" s="3">
+      <c r="M37" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O37" s="3">
         <f t="shared" si="8"/>
         <v>1.5584415584415584E-2</v>
       </c>
-      <c r="O37" s="5">
+      <c r="P37" s="5">
         <f t="shared" si="10"/>
         <v>12</v>
       </c>
-      <c r="P37" s="3">
+      <c r="Q37" s="3">
         <f t="shared" si="9"/>
         <v>7.7319587628865982E-3</v>
       </c>
-      <c r="Q37" s="5">
+      <c r="R37" s="5">
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="T37" s="1">
+      <c r="U37" s="1">
         <v>4898</v>
       </c>
-      <c r="U37" s="3">
+      <c r="V37" s="3">
         <v>-1.7805383022774329E-2</v>
       </c>
-      <c r="V37" s="3">
+      <c r="W37" s="3">
         <v>7.9162875341219296E-2</v>
       </c>
-      <c r="X37" s="1">
+      <c r="Y37" s="1">
         <v>4898</v>
       </c>
-      <c r="Y37" s="5">
+      <c r="Z37" s="5">
         <v>-43</v>
       </c>
-      <c r="Z37" s="5">
+      <c r="AA37" s="5">
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
@@ -6146,42 +6226,45 @@
       <c r="L38" s="2">
         <v>814</v>
       </c>
-      <c r="N38" s="3">
+      <c r="M38" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O38" s="3">
         <f t="shared" si="8"/>
         <v>7.4257425742574254E-3</v>
       </c>
-      <c r="O38" s="5">
+      <c r="P38" s="5">
         <f t="shared" si="10"/>
         <v>6</v>
       </c>
-      <c r="P38" s="3">
+      <c r="Q38" s="3">
         <f t="shared" si="9"/>
         <v>7.4257425742574254E-3</v>
       </c>
-      <c r="Q38" s="5">
+      <c r="R38" s="5">
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="T38" s="1">
+      <c r="U38" s="1">
         <v>5755</v>
-      </c>
-      <c r="U38" s="3">
-        <v>2.0581113801452784E-2</v>
       </c>
       <c r="V38" s="3">
         <v>2.0581113801452784E-2</v>
       </c>
-      <c r="X38" s="1">
+      <c r="W38" s="3">
+        <v>2.0581113801452784E-2</v>
+      </c>
+      <c r="Y38" s="1">
         <v>5755</v>
-      </c>
-      <c r="Y38" s="5">
-        <v>17</v>
       </c>
       <c r="Z38" s="5">
         <v>17</v>
       </c>
+      <c r="AA38" s="5">
+        <v>17</v>
+      </c>
     </row>
-    <row r="39" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>16</v>
       </c>
@@ -6211,42 +6294,45 @@
       <c r="L39" s="2">
         <v>843</v>
       </c>
-      <c r="N39" s="3">
+      <c r="M39" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O39" s="3">
         <f t="shared" si="8"/>
         <v>2.0581113801452784E-2</v>
       </c>
-      <c r="O39" s="5">
+      <c r="P39" s="5">
         <f t="shared" si="10"/>
         <v>17</v>
       </c>
-      <c r="P39" s="3">
+      <c r="Q39" s="3">
         <f t="shared" si="9"/>
         <v>2.0581113801452784E-2</v>
       </c>
-      <c r="Q39" s="5">
+      <c r="R39" s="5">
         <f t="shared" si="11"/>
         <v>17</v>
       </c>
-      <c r="T39" s="1">
+      <c r="U39" s="1">
         <v>6906</v>
-      </c>
-      <c r="U39" s="3">
-        <v>0</v>
       </c>
       <c r="V39" s="3">
         <v>0</v>
       </c>
-      <c r="X39" s="1">
+      <c r="W39" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="1">
         <v>9042</v>
-      </c>
-      <c r="Y39" s="5">
-        <v>0</v>
       </c>
       <c r="Z39" s="5">
         <v>0</v>
       </c>
+      <c r="AA39" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>4</v>
       </c>
@@ -6276,76 +6362,87 @@
       <c r="L40" s="2">
         <v>861</v>
       </c>
-      <c r="N40" s="3">
+      <c r="M40" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O40" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3">
+      <c r="P40" s="5">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="3">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Q40" s="3"/>
-      <c r="T40" s="1">
+      <c r="R40" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="U40" s="1">
         <v>9042</v>
-      </c>
-      <c r="U40" s="3">
-        <v>0</v>
       </c>
       <c r="V40" s="3">
         <v>0</v>
       </c>
-      <c r="X40" s="1">
+      <c r="W40" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="1">
         <v>9796</v>
-      </c>
-      <c r="Y40" s="5">
-        <v>69</v>
       </c>
       <c r="Z40" s="5">
         <v>69</v>
       </c>
+      <c r="AA40" s="5">
+        <v>69</v>
+      </c>
     </row>
-    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="T41" s="1">
+    <row r="41" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="M41" s="4"/>
+      <c r="U41" s="1">
         <v>9796</v>
-      </c>
-      <c r="U41" s="3">
-        <v>2.7111984282907661E-2</v>
       </c>
       <c r="V41" s="3">
         <v>2.7111984282907661E-2</v>
       </c>
-      <c r="X41" s="1">
+      <c r="W41" s="3">
+        <v>2.7111984282907661E-2</v>
+      </c>
+      <c r="Y41" s="1">
         <v>13563</v>
-      </c>
-      <c r="Y41" s="5">
-        <v>7</v>
       </c>
       <c r="Z41" s="5">
         <v>7</v>
       </c>
+      <c r="AA41" s="5">
+        <v>7</v>
+      </c>
     </row>
-    <row r="42" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="T42" s="1">
+    <row r="42" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="M42" s="4"/>
+      <c r="U42" s="1">
         <v>13563</v>
-      </c>
-      <c r="U42" s="3">
-        <v>1.7114914425427872E-3</v>
       </c>
       <c r="V42" s="3">
         <v>1.7114914425427872E-3</v>
       </c>
-      <c r="X42" s="1">
+      <c r="W42" s="3">
+        <v>1.7114914425427872E-3</v>
+      </c>
+      <c r="Y42" s="1">
         <v>14694</v>
-      </c>
-      <c r="Y42" s="5">
-        <v>21</v>
       </c>
       <c r="Z42" s="5">
         <v>21</v>
       </c>
+      <c r="AA42" s="5">
+        <v>21</v>
+      </c>
     </row>
-    <row r="43" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
       <c r="F43" s="1" t="s">
         <v>5</v>
@@ -6364,30 +6461,31 @@
       <c r="L43" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N43" s="3"/>
+      <c r="M43" s="4"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
-      <c r="T43" s="1">
+      <c r="R43" s="3"/>
+      <c r="U43" s="1">
         <v>14694</v>
-      </c>
-      <c r="U43" s="3">
-        <v>7.9787234042553185E-3</v>
       </c>
       <c r="V43" s="3">
         <v>7.9787234042553185E-3</v>
       </c>
-      <c r="X43" s="1">
+      <c r="W43" s="3">
+        <v>7.9787234042553185E-3</v>
+      </c>
+      <c r="Y43" s="1">
         <v>18084</v>
-      </c>
-      <c r="Y43" s="5">
-        <v>3</v>
       </c>
       <c r="Z43" s="5">
         <v>3</v>
       </c>
+      <c r="AA43" s="5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="44" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>0</v>
       </c>
@@ -6417,42 +6515,45 @@
       <c r="L44" s="2">
         <v>14003</v>
       </c>
-      <c r="N44" s="3">
-        <f t="shared" ref="N44:N49" si="12">(L44-I44)/I44</f>
+      <c r="M44" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O44" s="3">
+        <f t="shared" ref="O44:O49" si="12">(L44-I44)/I44</f>
         <v>3.727331374095047E-3</v>
       </c>
-      <c r="O44" s="5">
+      <c r="P44" s="5">
         <f>L44-I44</f>
         <v>52</v>
       </c>
-      <c r="P44" s="3">
-        <f t="shared" ref="P44:P49" si="13">(L44-J44)/J44</f>
+      <c r="Q44" s="3">
+        <f t="shared" ref="Q44:Q49" si="13">(L44-J44)/J44</f>
         <v>3.727331374095047E-3</v>
       </c>
-      <c r="Q44" s="5">
+      <c r="R44" s="5">
         <f>L44-J44</f>
         <v>52</v>
       </c>
-      <c r="T44" s="1">
+      <c r="U44" s="1">
         <v>18084</v>
-      </c>
-      <c r="U44" s="3">
-        <v>7.2709646146388749E-4</v>
       </c>
       <c r="V44" s="3">
         <v>7.2709646146388749E-4</v>
       </c>
-      <c r="X44" s="1">
+      <c r="W44" s="3">
+        <v>7.2709646146388749E-4</v>
+      </c>
+      <c r="Y44" s="1">
         <v>19020</v>
-      </c>
-      <c r="Y44" s="5">
-        <v>52</v>
       </c>
       <c r="Z44" s="5">
         <v>52</v>
       </c>
+      <c r="AA44" s="5">
+        <v>52</v>
+      </c>
     </row>
-    <row r="45" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>1</v>
       </c>
@@ -6482,42 +6583,45 @@
       <c r="L45" s="2">
         <v>15176</v>
       </c>
-      <c r="N45" s="3">
+      <c r="M45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O45" s="3">
         <f t="shared" si="12"/>
         <v>1.0049916805324459E-2</v>
       </c>
-      <c r="O45" s="5">
-        <f t="shared" ref="O45:O47" si="14">L45-I45</f>
+      <c r="P45" s="5">
+        <f t="shared" ref="P45:P47" si="14">L45-I45</f>
         <v>151</v>
       </c>
-      <c r="P45" s="3">
+      <c r="Q45" s="3">
         <f t="shared" si="13"/>
         <v>1.0049916805324459E-2</v>
       </c>
-      <c r="Q45" s="5">
-        <f t="shared" ref="Q45:Q47" si="15">L45-J45</f>
+      <c r="R45" s="5">
+        <f t="shared" ref="R45:R47" si="15">L45-J45</f>
         <v>151</v>
       </c>
-      <c r="T45" s="1">
+      <c r="U45" s="1">
         <v>19020</v>
-      </c>
-      <c r="U45" s="3">
-        <v>3.727331374095047E-3</v>
       </c>
       <c r="V45" s="3">
         <v>3.727331374095047E-3</v>
       </c>
-      <c r="X45" s="1">
+      <c r="W45" s="3">
+        <v>3.727331374095047E-3</v>
+      </c>
+      <c r="Y45" s="1">
         <v>19592</v>
-      </c>
-      <c r="Y45" s="5">
-        <v>6</v>
       </c>
       <c r="Z45" s="5">
         <v>6</v>
       </c>
+      <c r="AA45" s="5">
+        <v>6</v>
+      </c>
     </row>
-    <row r="46" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>2</v>
       </c>
@@ -6547,42 +6651,45 @@
       <c r="L46" s="2">
         <v>15277</v>
       </c>
-      <c r="N46" s="3">
+      <c r="M46" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O46" s="3">
         <f t="shared" si="12"/>
         <v>1.1721854304635761E-2</v>
       </c>
-      <c r="O46" s="5">
+      <c r="P46" s="5">
         <f t="shared" si="14"/>
         <v>177</v>
       </c>
-      <c r="P46" s="3">
+      <c r="Q46" s="3">
         <f t="shared" si="13"/>
         <v>1.1721854304635761E-2</v>
       </c>
-      <c r="Q46" s="5">
+      <c r="R46" s="5">
         <f t="shared" si="15"/>
         <v>177</v>
       </c>
-      <c r="T46" s="1">
+      <c r="U46" s="1">
         <v>19592</v>
-      </c>
-      <c r="U46" s="3">
-        <v>2.216475803472479E-3</v>
       </c>
       <c r="V46" s="3">
         <v>2.216475803472479E-3</v>
       </c>
-      <c r="X46" s="1">
+      <c r="W46" s="3">
+        <v>2.216475803472479E-3</v>
+      </c>
+      <c r="Y46" s="1">
         <v>22605</v>
-      </c>
-      <c r="Y46" s="5">
-        <v>1</v>
       </c>
       <c r="Z46" s="5">
         <v>1</v>
       </c>
+      <c r="AA46" s="5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="47" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
         <v>3</v>
       </c>
@@ -6612,42 +6719,45 @@
       <c r="L47" s="2">
         <v>15683</v>
       </c>
-      <c r="N47" s="3">
+      <c r="M47" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O47" s="3">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="O47" s="5">
+      <c r="P47" s="5">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="P47" s="3">
+      <c r="Q47" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="Q47" s="5">
+      <c r="R47" s="5">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="T47" s="1">
+      <c r="U47" s="1">
         <v>22605</v>
-      </c>
-      <c r="U47" s="3">
-        <v>2.4021138601969732E-4</v>
       </c>
       <c r="V47" s="3">
         <v>2.4021138601969732E-4</v>
       </c>
-      <c r="X47" s="1">
+      <c r="W47" s="3">
+        <v>2.4021138601969732E-4</v>
+      </c>
+      <c r="Y47" s="1">
         <v>24490</v>
-      </c>
-      <c r="Y47" s="5">
-        <v>18</v>
       </c>
       <c r="Z47" s="5">
         <v>18</v>
       </c>
+      <c r="AA47" s="5">
+        <v>18</v>
+      </c>
     </row>
-    <row r="48" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
         <v>16</v>
       </c>
@@ -6669,36 +6779,37 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-      <c r="N48" s="3" t="e">
+      <c r="M48" s="4"/>
+      <c r="O48" s="3" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O48" s="5"/>
-      <c r="P48" s="3" t="e">
+      <c r="P48" s="5"/>
+      <c r="Q48" s="3" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q48" s="5"/>
-      <c r="T48" s="1">
+      <c r="R48" s="5"/>
+      <c r="U48" s="1">
         <v>24490</v>
-      </c>
-      <c r="U48" s="3">
-        <v>6.4700000000000001E-3</v>
       </c>
       <c r="V48" s="3">
         <v>6.4700000000000001E-3</v>
       </c>
-      <c r="X48" s="1">
+      <c r="W48" s="3">
+        <v>6.4700000000000001E-3</v>
+      </c>
+      <c r="Y48" s="1">
         <v>38040</v>
-      </c>
-      <c r="Y48" s="5">
-        <v>151</v>
       </c>
       <c r="Z48" s="5">
         <v>151</v>
       </c>
+      <c r="AA48" s="5">
+        <v>151</v>
+      </c>
     </row>
-    <row r="49" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
@@ -6720,572 +6831,573 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
-      <c r="N49" s="3" t="e">
+      <c r="M49" s="4"/>
+      <c r="O49" s="3" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3" t="e">
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q49" s="3"/>
-      <c r="T49" s="1">
+      <c r="R49" s="3"/>
+      <c r="U49" s="1">
         <v>38040</v>
-      </c>
-      <c r="U49" s="3">
-        <v>1.0049916805324459E-2</v>
       </c>
       <c r="V49" s="3">
         <v>1.0049916805324459E-2</v>
       </c>
-      <c r="X49" s="1">
+      <c r="W49" s="3">
+        <v>1.0049916805324459E-2</v>
+      </c>
+      <c r="Y49" s="1">
         <v>57060</v>
-      </c>
-      <c r="Y49" s="5">
-        <v>177</v>
       </c>
       <c r="Z49" s="5">
         <v>177</v>
       </c>
+      <c r="AA49" s="5">
+        <v>177</v>
+      </c>
     </row>
-    <row r="50" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="T50" s="1">
+    <row r="50" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="U50" s="1">
         <v>57060</v>
-      </c>
-      <c r="U50" s="3">
-        <v>1.1721854304635761E-2</v>
       </c>
       <c r="V50" s="3">
         <v>1.1721854304635761E-2</v>
       </c>
-      <c r="X50" s="1">
+      <c r="W50" s="3">
+        <v>1.1721854304635761E-2</v>
+      </c>
+      <c r="Y50" s="1">
         <v>76080</v>
-      </c>
-      <c r="Y50" s="5">
-        <v>0</v>
       </c>
       <c r="Z50" s="5">
         <v>0</v>
       </c>
+      <c r="AA50" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="T51" s="1">
+    <row r="51" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="U51" s="1">
         <v>76080</v>
-      </c>
-      <c r="U51" s="3">
-        <v>0</v>
       </c>
       <c r="V51" s="3">
         <v>0</v>
       </c>
-      <c r="X51" s="1"/>
-      <c r="Y51" s="5"/>
+      <c r="W51" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="1"/>
       <c r="Z51" s="5"/>
+      <c r="AA51" s="5"/>
     </row>
-    <row r="52" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="X52" s="1"/>
-      <c r="Y52" s="3"/>
+    <row r="52" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="Y52" s="1"/>
       <c r="Z52" s="3"/>
+      <c r="AA52" s="3"/>
     </row>
-    <row r="60" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="T60" s="1">
+    <row r="60" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="U60" s="1">
         <v>1536</v>
       </c>
-      <c r="U60" s="3">
+      <c r="V60" s="3">
         <v>0</v>
       </c>
-      <c r="V60" s="3">
+      <c r="W60" s="3">
         <v>1.9469026548672566E-2</v>
       </c>
-      <c r="X60" s="1">
+      <c r="Y60" s="1">
         <v>1536</v>
       </c>
-      <c r="Y60" s="5">
+      <c r="Z60" s="5">
         <v>0</v>
       </c>
-      <c r="Z60" s="5">
+      <c r="AA60" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="T61" s="1">
+    <row r="61" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="U61" s="1">
         <v>2302</v>
       </c>
-      <c r="U61" s="3">
+      <c r="V61" s="3">
         <v>-1.8439716312056736E-2</v>
       </c>
-      <c r="V61" s="3">
+      <c r="W61" s="3">
         <v>2.3668639053254437E-2</v>
       </c>
-      <c r="X61" s="1">
+      <c r="Y61" s="1">
         <v>2302</v>
       </c>
-      <c r="Y61" s="5">
+      <c r="Z61" s="5">
         <v>-13</v>
       </c>
-      <c r="Z61" s="5">
+      <c r="AA61" s="5">
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="T62" s="1">
+    <row r="62" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="U62" s="1">
         <v>3072</v>
       </c>
-      <c r="U62" s="3">
+      <c r="V62" s="3">
         <v>0</v>
       </c>
-      <c r="V62" s="3">
+      <c r="W62" s="3">
         <v>5.0590219224283303E-3</v>
       </c>
-      <c r="X62" s="1">
+      <c r="Y62" s="1">
         <v>3072</v>
       </c>
-      <c r="Y62" s="5">
+      <c r="Z62" s="5">
         <v>0</v>
       </c>
-      <c r="Z62" s="5">
+      <c r="AA62" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="T63" s="1">
+    <row r="63" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="U63" s="1">
         <v>4604</v>
       </c>
-      <c r="U63" s="3">
+      <c r="V63" s="3">
         <v>-1.3280212483399733E-3</v>
       </c>
-      <c r="V63" s="3">
+      <c r="W63" s="3">
         <v>1.3315579227696406E-3</v>
       </c>
-      <c r="X63" s="1">
+      <c r="Y63" s="1">
         <v>4604</v>
       </c>
-      <c r="Y63" s="5">
+      <c r="Z63" s="5">
         <v>-1</v>
       </c>
-      <c r="Z63" s="5">
+      <c r="AA63" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="T64" s="1">
+    <row r="64" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="U64" s="1">
         <v>6144</v>
       </c>
-      <c r="U64" s="3">
+      <c r="V64" s="3">
         <v>8.2781456953642391E-3</v>
       </c>
-      <c r="V64" s="3">
+      <c r="W64" s="3">
         <v>2.1812080536912751E-2</v>
       </c>
-      <c r="X64" s="1">
+      <c r="Y64" s="1">
         <v>6144</v>
       </c>
-      <c r="Y64" s="5">
+      <c r="Z64" s="5">
         <v>5</v>
       </c>
-      <c r="Z64" s="5">
+      <c r="AA64" s="5">
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T65" s="1">
+    <row r="65" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U65" s="1">
         <v>9042</v>
       </c>
-      <c r="U65" s="3">
+      <c r="V65" s="3">
         <v>-8.9175130047064646E-3</v>
       </c>
-      <c r="V65" s="3">
+      <c r="W65" s="3">
         <v>0</v>
       </c>
-      <c r="X65" s="1">
+      <c r="Y65" s="1">
         <v>9042</v>
       </c>
-      <c r="Y65" s="5">
+      <c r="Z65" s="5">
         <v>-36</v>
       </c>
-      <c r="Z65" s="5">
+      <c r="AA65" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T66" s="1">
+    <row r="66" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U66" s="1">
         <v>9208</v>
       </c>
-      <c r="U66" s="3">
+      <c r="V66" s="3">
         <v>7.7319587628865982E-3</v>
       </c>
-      <c r="V66" s="3">
+      <c r="W66" s="3">
         <v>1.5584415584415584E-2</v>
       </c>
-      <c r="X66" s="1">
+      <c r="Y66" s="1">
         <v>9208</v>
       </c>
-      <c r="Y66" s="5">
+      <c r="Z66" s="5">
         <v>6</v>
       </c>
-      <c r="Z66" s="5">
+      <c r="AA66" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T67" s="1">
+    <row r="67" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U67" s="1">
         <v>9796</v>
       </c>
-      <c r="U67" s="3">
+      <c r="V67" s="3">
         <v>-1.7805383022774329E-2</v>
       </c>
-      <c r="V67" s="3">
+      <c r="W67" s="3">
         <v>7.9162875341219296E-2</v>
       </c>
-      <c r="X67" s="1">
+      <c r="Y67" s="1">
         <v>9796</v>
       </c>
-      <c r="Y67" s="5">
+      <c r="Z67" s="5">
         <v>-43</v>
       </c>
-      <c r="Z67" s="5">
+      <c r="AA67" s="5">
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T68" s="1">
+    <row r="68" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U68" s="1">
         <v>12288</v>
       </c>
-      <c r="U68" s="3">
+      <c r="V68" s="3">
         <v>3.2362459546925568E-3</v>
       </c>
-      <c r="V68" s="3">
+      <c r="W68" s="3">
         <v>1.9736842105263157E-2</v>
       </c>
-      <c r="X68" s="1">
+      <c r="Y68" s="1">
         <v>12288</v>
       </c>
-      <c r="Y68" s="5">
+      <c r="Z68" s="5">
         <v>2</v>
       </c>
-      <c r="Z68" s="5">
+      <c r="AA68" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T69" s="1">
+    <row r="69" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U69" s="1">
         <v>18084</v>
-      </c>
-      <c r="U69" s="3">
-        <v>0</v>
       </c>
       <c r="V69" s="3">
         <v>0</v>
       </c>
-      <c r="X69" s="1">
+      <c r="W69" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y69" s="1">
         <v>18084</v>
-      </c>
-      <c r="Y69" s="5">
-        <v>0</v>
       </c>
       <c r="Z69" s="5">
         <v>0</v>
       </c>
+      <c r="AA69" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T70" s="1">
+    <row r="70" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U70" s="1">
         <v>18416</v>
-      </c>
-      <c r="U70" s="3">
-        <v>7.4257425742574254E-3</v>
       </c>
       <c r="V70" s="3">
         <v>7.4257425742574254E-3</v>
       </c>
-      <c r="X70" s="1">
+      <c r="W70" s="3">
+        <v>7.4257425742574254E-3</v>
+      </c>
+      <c r="Y70" s="1">
         <v>18416</v>
-      </c>
-      <c r="Y70" s="5">
-        <v>6</v>
       </c>
       <c r="Z70" s="5">
         <v>6</v>
       </c>
+      <c r="AA70" s="5">
+        <v>6</v>
+      </c>
     </row>
-    <row r="71" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T71" s="1">
+    <row r="71" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U71" s="1">
         <v>19592</v>
-      </c>
-      <c r="U71" s="3">
-        <v>2.7111984282907661E-2</v>
       </c>
       <c r="V71" s="3">
         <v>2.7111984282907661E-2</v>
       </c>
-      <c r="X71" s="1">
+      <c r="W71" s="3">
+        <v>2.7111984282907661E-2</v>
+      </c>
+      <c r="Y71" s="1">
         <v>19592</v>
-      </c>
-      <c r="Y71" s="5">
-        <v>69</v>
       </c>
       <c r="Z71" s="5">
         <v>69</v>
       </c>
+      <c r="AA71" s="5">
+        <v>69</v>
+      </c>
     </row>
-    <row r="72" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T72" s="1">
+    <row r="72" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U72" s="1">
         <v>24576</v>
-      </c>
-      <c r="U72" s="3">
-        <v>0</v>
       </c>
       <c r="V72" s="3">
         <v>0</v>
       </c>
-      <c r="X72" s="1">
+      <c r="W72" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y72" s="1">
         <v>24576</v>
-      </c>
-      <c r="Y72" s="5">
-        <v>0</v>
       </c>
       <c r="Z72" s="5">
         <v>0</v>
       </c>
+      <c r="AA72" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="73" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T73" s="1">
+    <row r="73" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U73" s="1">
         <v>36168</v>
-      </c>
-      <c r="U73" s="3">
-        <v>1.7114914425427872E-3</v>
       </c>
       <c r="V73" s="3">
         <v>1.7114914425427872E-3</v>
       </c>
-      <c r="X73" s="1">
+      <c r="W73" s="3">
+        <v>1.7114914425427872E-3</v>
+      </c>
+      <c r="Y73" s="1">
         <v>36168</v>
-      </c>
-      <c r="Y73" s="5">
-        <v>7</v>
       </c>
       <c r="Z73" s="5">
         <v>7</v>
       </c>
+      <c r="AA73" s="5">
+        <v>7</v>
+      </c>
     </row>
-    <row r="74" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T74" s="1">
+    <row r="74" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U74" s="1">
         <v>36832</v>
-      </c>
-      <c r="U74" s="3">
-        <v>2.0581113801452784E-2</v>
       </c>
       <c r="V74" s="3">
         <v>2.0581113801452784E-2</v>
       </c>
-      <c r="X74" s="1">
+      <c r="W74" s="3">
+        <v>2.0581113801452784E-2</v>
+      </c>
+      <c r="Y74" s="1">
         <v>36832</v>
-      </c>
-      <c r="Y74" s="5">
-        <v>17</v>
       </c>
       <c r="Z74" s="5">
         <v>17</v>
       </c>
+      <c r="AA74" s="5">
+        <v>17</v>
+      </c>
     </row>
-    <row r="75" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T75" s="1">
+    <row r="75" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U75" s="1">
         <v>38040</v>
-      </c>
-      <c r="U75" s="3">
-        <v>3.727331374095047E-3</v>
       </c>
       <c r="V75" s="3">
         <v>3.727331374095047E-3</v>
       </c>
-      <c r="X75" s="1">
+      <c r="W75" s="3">
+        <v>3.727331374095047E-3</v>
+      </c>
+      <c r="Y75" s="1">
         <v>38040</v>
-      </c>
-      <c r="Y75" s="5">
-        <v>52</v>
       </c>
       <c r="Z75" s="5">
         <v>52</v>
       </c>
+      <c r="AA75" s="5">
+        <v>52</v>
+      </c>
     </row>
-    <row r="76" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T76" s="1">
+    <row r="76" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U76" s="1">
         <v>39184</v>
-      </c>
-      <c r="U76" s="3">
-        <v>7.9787234042553185E-3</v>
       </c>
       <c r="V76" s="3">
         <v>7.9787234042553185E-3</v>
       </c>
-      <c r="X76" s="1">
+      <c r="W76" s="3">
+        <v>7.9787234042553185E-3</v>
+      </c>
+      <c r="Y76" s="1">
         <v>39184</v>
-      </c>
-      <c r="Y76" s="5">
-        <v>21</v>
       </c>
       <c r="Z76" s="5">
         <v>21</v>
       </c>
+      <c r="AA76" s="5">
+        <v>21</v>
+      </c>
     </row>
-    <row r="77" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T77" s="1">
+    <row r="77" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U77" s="1">
         <v>72336</v>
-      </c>
-      <c r="U77" s="3">
-        <v>7.2709646146388749E-4</v>
       </c>
       <c r="V77" s="3">
         <v>7.2709646146388749E-4</v>
       </c>
-      <c r="X77" s="1">
+      <c r="W77" s="3">
+        <v>7.2709646146388749E-4</v>
+      </c>
+      <c r="Y77" s="1">
         <v>72336</v>
-      </c>
-      <c r="Y77" s="5">
-        <v>3</v>
       </c>
       <c r="Z77" s="5">
         <v>3</v>
       </c>
+      <c r="AA77" s="5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="78" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T78" s="1">
+    <row r="78" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U78" s="1">
         <v>73664</v>
-      </c>
-      <c r="U78" s="3">
-        <v>0</v>
       </c>
       <c r="V78" s="3">
         <v>0</v>
       </c>
-      <c r="X78" s="1">
+      <c r="W78" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y78" s="1">
         <v>76080</v>
-      </c>
-      <c r="Y78" s="5">
-        <v>151</v>
       </c>
       <c r="Z78" s="5">
         <v>151</v>
       </c>
+      <c r="AA78" s="5">
+        <v>151</v>
+      </c>
     </row>
-    <row r="79" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T79" s="1">
+    <row r="79" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U79" s="1">
         <v>76080</v>
-      </c>
-      <c r="U79" s="3">
-        <v>1.0049916805324459E-2</v>
       </c>
       <c r="V79" s="3">
         <v>1.0049916805324459E-2</v>
       </c>
-      <c r="X79" s="1">
+      <c r="W79" s="3">
+        <v>1.0049916805324459E-2</v>
+      </c>
+      <c r="Y79" s="1">
         <v>78368</v>
-      </c>
-      <c r="Y79" s="5">
-        <v>6</v>
       </c>
       <c r="Z79" s="5">
         <v>6</v>
       </c>
+      <c r="AA79" s="5">
+        <v>6</v>
+      </c>
     </row>
-    <row r="80" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T80" s="1">
+    <row r="80" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U80" s="1">
         <v>78368</v>
-      </c>
-      <c r="U80" s="3">
-        <v>2.216475803472479E-3</v>
       </c>
       <c r="V80" s="3">
         <v>2.216475803472479E-3</v>
       </c>
-      <c r="X80" s="1">
+      <c r="W80" s="3">
+        <v>2.216475803472479E-3</v>
+      </c>
+      <c r="Y80" s="1">
         <v>144672</v>
-      </c>
-      <c r="Y80" s="5">
-        <v>1</v>
       </c>
       <c r="Z80" s="5">
         <v>1</v>
       </c>
+      <c r="AA80" s="5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T81" s="1">
+    <row r="81" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U81" s="1">
         <v>144672</v>
-      </c>
-      <c r="U81" s="3">
-        <v>2.4021138601969732E-4</v>
       </c>
       <c r="V81" s="3">
         <v>2.4021138601969732E-4</v>
       </c>
-      <c r="X81" s="1">
+      <c r="W81" s="3">
+        <v>2.4021138601969732E-4</v>
+      </c>
+      <c r="Y81" s="1">
         <v>152160</v>
-      </c>
-      <c r="Y81" s="5">
-        <v>177</v>
       </c>
       <c r="Z81" s="5">
         <v>177</v>
       </c>
+      <c r="AA81" s="5">
+        <v>177</v>
+      </c>
     </row>
-    <row r="82" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T82" s="1">
+    <row r="82" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U82" s="1">
         <v>152160</v>
-      </c>
-      <c r="U82" s="3">
-        <v>1.1721854304635761E-2</v>
       </c>
       <c r="V82" s="3">
         <v>1.1721854304635761E-2</v>
       </c>
-      <c r="X82" s="1">
+      <c r="W82" s="3">
+        <v>1.1721854304635761E-2</v>
+      </c>
+      <c r="Y82" s="1">
         <v>156736</v>
-      </c>
-      <c r="Y82" s="5">
-        <v>18</v>
       </c>
       <c r="Z82" s="5">
         <v>18</v>
       </c>
+      <c r="AA82" s="5">
+        <v>18</v>
+      </c>
     </row>
-    <row r="83" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T83" s="1">
+    <row r="83" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U83" s="1">
         <v>156736</v>
-      </c>
-      <c r="U83" s="3">
-        <v>6.4701653486700216E-3</v>
       </c>
       <c r="V83" s="3">
         <v>6.4701653486700216E-3</v>
       </c>
-      <c r="X83" s="1">
+      <c r="W83" s="3">
+        <v>6.4701653486700216E-3</v>
+      </c>
+      <c r="Y83" s="1">
         <v>304320</v>
-      </c>
-      <c r="Y83" s="5">
-        <v>0</v>
       </c>
       <c r="Z83" s="5">
         <v>0</v>
       </c>
+      <c r="AA83" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="84" spans="20:26" x14ac:dyDescent="0.25">
-      <c r="T84" s="1">
+    <row r="84" spans="21:27" x14ac:dyDescent="0.25">
+      <c r="U84" s="1">
         <v>304320</v>
-      </c>
-      <c r="U84" s="3">
-        <v>0</v>
       </c>
       <c r="V84" s="3">
         <v>0</v>
       </c>
+      <c r="W84" s="3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="X60:Z83">
-    <sortCondition ref="X60"/>
+  <sortState ref="Y60:AA83">
+    <sortCondition ref="Y60"/>
   </sortState>
   <mergeCells count="2">
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="O4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Results, version 19/06 16h31
</commit_message>
<xml_diff>
--- a/Results_CG.xlsx
+++ b/Results_CG.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3A506777-5A44-4788-98FD-3AD16CDA5BBD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{46702E93-70A5-4EEA-8D22-5A66196ED81F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:AC84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="S51" sqref="S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2543,14 +2543,29 @@
       <c r="L47" s="10">
         <v>15683</v>
       </c>
+      <c r="M47" s="2">
+        <v>15737</v>
+      </c>
       <c r="N47" s="4" t="s">
         <v>45</v>
       </c>
       <c r="O47" s="7"/>
-      <c r="Q47" s="3"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="3"/>
-      <c r="T47" s="5"/>
+      <c r="Q47" s="3">
+        <f t="shared" ref="Q47" si="8">(M47-I47)/I47</f>
+        <v>3.443218771918638E-3</v>
+      </c>
+      <c r="R47" s="5">
+        <f t="shared" ref="R47" si="9">M47-I47</f>
+        <v>54</v>
+      </c>
+      <c r="S47" s="3">
+        <f t="shared" ref="S47" si="10">(M47-J47)/J47</f>
+        <v>3.443218771918638E-3</v>
+      </c>
+      <c r="T47" s="5">
+        <f t="shared" ref="T47" si="11">M47-J47</f>
+        <v>54</v>
+      </c>
       <c r="W47" s="1"/>
       <c r="X47" s="3"/>
       <c r="Y47" s="3"/>

</xml_diff>

<commit_message>
Results, version 20/06 9h40
</commit_message>
<xml_diff>
--- a/Results_CG.xlsx
+++ b/Results_CG.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{46702E93-70A5-4EEA-8D22-5A66196ED81F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{19E1AADA-9DEE-49FC-A6A4-7DA9C0E6EA98}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="64">
   <si>
     <t>Instance name</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>42m45s</t>
+  </si>
+  <si>
+    <t>0,04s</t>
+  </si>
+  <si>
+    <t>7s</t>
   </si>
 </sst>
 </file>
@@ -263,7 +269,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -296,6 +302,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -583,7 +592,7 @@
   <dimension ref="C3:AC84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="S51" sqref="S51"/>
+      <selection activeCell="J36" sqref="J36:M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,14 +625,14 @@
       </c>
     </row>
     <row r="4" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="Q4" s="12" t="s">
+      <c r="Q4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12" t="s">
+      <c r="R4" s="13"/>
+      <c r="S4" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="T4" s="12"/>
+      <c r="T4" s="13"/>
       <c r="V4" t="s">
         <v>38</v>
       </c>
@@ -1930,7 +1939,9 @@
       <c r="N35" s="2">
         <v>705</v>
       </c>
-      <c r="O35" s="7"/>
+      <c r="O35" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="Q35" s="3">
         <f t="shared" si="0"/>
         <v>4.2899408284023666E-2</v>
@@ -1975,22 +1986,24 @@
       <c r="I36" s="9">
         <v>751</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J36" s="12">
         <v>753</v>
       </c>
-      <c r="K36" s="9" t="s">
+      <c r="K36" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L36" s="9">
+      <c r="L36" s="12">
         <v>752</v>
       </c>
-      <c r="M36" s="2">
+      <c r="M36" s="12">
         <v>753</v>
       </c>
-      <c r="N36" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O36" s="7"/>
+      <c r="N36" s="2">
+        <v>768</v>
+      </c>
+      <c r="O36" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="Q36" s="3">
         <f t="shared" si="0"/>
         <v>2.6631158455392811E-3</v>
@@ -2369,19 +2382,19 @@
         <v>59</v>
       </c>
       <c r="Q44" s="3">
-        <f t="shared" ref="Q41:Q46" si="4">(M44-I44)/I44</f>
+        <f t="shared" ref="Q44:Q46" si="4">(M44-I44)/I44</f>
         <v>5.8060354096480535E-3</v>
       </c>
       <c r="R44" s="5">
-        <f t="shared" ref="R41:R46" si="5">M44-I44</f>
+        <f t="shared" ref="R44:R46" si="5">M44-I44</f>
         <v>81</v>
       </c>
       <c r="S44" s="3">
-        <f t="shared" ref="S41:S46" si="6">(M44-J44)/J44</f>
+        <f t="shared" ref="S44:S46" si="6">(M44-J44)/J44</f>
         <v>5.8060354096480535E-3</v>
       </c>
       <c r="T44" s="5">
-        <f t="shared" ref="T41:T46" si="7">M44-J44</f>
+        <f t="shared" ref="T44:T46" si="7">M44-J44</f>
         <v>81</v>
       </c>
       <c r="W44" s="1"/>

</xml_diff>

<commit_message>
Results version 21/06 16h40
</commit_message>
<xml_diff>
--- a/Results_CG.xlsx
+++ b/Results_CG.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2C9CFC50-ECE7-40A8-8CD7-D91AA778FDF1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{157001E6-BFBC-4673-A483-48826F8FD31B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="77">
   <si>
     <t>Instance name</t>
   </si>
@@ -221,6 +221,36 @@
   </si>
   <si>
     <t>Not available yet</t>
+  </si>
+  <si>
+    <t>843**</t>
+  </si>
+  <si>
+    <t>817**</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Post-processing lv2 takes too much time</t>
+  </si>
+  <si>
+    <t>Imbalanced data (11,5%)</t>
+  </si>
+  <si>
+    <t>Post-processing lv2 takes too much time (32m)</t>
+  </si>
+  <si>
+    <t>CART + pp1</t>
+  </si>
+  <si>
+    <t>CART + pp2</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Post-processing lv2 takes too much time (11m)</t>
   </si>
 </sst>
 </file>
@@ -230,7 +260,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,8 +281,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +299,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -274,11 +316,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -320,8 +363,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -601,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:AD84"/>
+  <dimension ref="C3:AG84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
+      <selection activeCell="S50" sqref="S50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,37 +673,40 @@
     <col min="11" max="12" width="11.140625" customWidth="1"/>
     <col min="13" max="13" width="20.28515625" style="6" customWidth="1"/>
     <col min="14" max="14" width="20.28515625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" customWidth="1"/>
-    <col min="18" max="19" width="19.7109375" customWidth="1"/>
-    <col min="20" max="21" width="17.28515625" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" customWidth="1"/>
-    <col min="25" max="25" width="12.85546875" customWidth="1"/>
-    <col min="27" max="27" width="34.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="14" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" style="14" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" customWidth="1"/>
+    <col min="19" max="19" width="46.5703125" customWidth="1"/>
+    <col min="21" max="22" width="19.7109375" customWidth="1"/>
+    <col min="23" max="24" width="17.28515625" customWidth="1"/>
+    <col min="25" max="25" width="12.5703125" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" customWidth="1"/>
+    <col min="30" max="30" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="W3" t="s">
+    <row r="3" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="Z3" t="s">
         <v>15</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AD3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="R4" s="14" t="s">
+    <row r="4" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="U4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14" t="s">
+      <c r="V4" s="15"/>
+      <c r="W4" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="14"/>
-      <c r="W4" t="s">
+      <c r="X4" s="15"/>
+      <c r="Z4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>5</v>
@@ -679,21 +735,30 @@
       <c r="N5" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="Q5" s="1"/>
-      <c r="W5" t="s">
+      <c r="S5" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="T5" s="1"/>
+      <c r="Z5" t="s">
         <v>39</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AD5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,34 +797,43 @@
       <c r="N6" s="2">
         <v>4037</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q6" s="2">
         <v>4037</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="R6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="3">
-        <f>(M6-I6)/I6</f>
+      <c r="S6" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="3">
+        <f>(N6-I6)/I6</f>
         <v>8.9977505623594096E-3</v>
       </c>
-      <c r="S6" s="5">
+      <c r="V6" s="5">
         <f>M6-I6</f>
         <v>36</v>
       </c>
-      <c r="T6" s="3">
-        <f>(M6-J6)/J6</f>
+      <c r="W6" s="3">
+        <f>(N6-J6)/J6</f>
         <v>0</v>
       </c>
-      <c r="U6" s="5">
+      <c r="X6" s="5">
         <f>M6-J6</f>
         <v>0</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AD6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
@@ -795,34 +869,38 @@
       <c r="N7" s="2">
         <v>4075</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q7" s="2">
         <v>4075</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="R7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="3">
-        <f t="shared" ref="R7:R40" si="0">(M7-I7)/I7</f>
+      <c r="S7" s="15"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="3">
+        <f t="shared" ref="U7:U10" si="0">(N7-I7)/I7</f>
+        <v>4.9103854652590229E-4</v>
+      </c>
+      <c r="V7" s="5">
+        <f t="shared" ref="V7:V40" si="1">M7-I7</f>
         <v>0</v>
       </c>
-      <c r="S7" s="5">
-        <f t="shared" ref="S7:S40" si="1">M7-I7</f>
+      <c r="W7" s="3">
+        <f t="shared" ref="W7:W10" si="2">(N7-J7)/J7</f>
+        <v>4.9103854652590229E-4</v>
+      </c>
+      <c r="X7" s="5">
+        <f t="shared" ref="X7:X40" si="3">M7-J7</f>
         <v>0</v>
       </c>
-      <c r="T7" s="3">
-        <f t="shared" ref="T7:T40" si="2">(M7-J7)/J7</f>
-        <v>0</v>
-      </c>
-      <c r="U7" s="5">
-        <f t="shared" ref="U7:U40" si="3">M7-J7</f>
-        <v>0</v>
-      </c>
-      <c r="AA7" t="s">
+      <c r="AD7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
@@ -858,31 +936,38 @@
       <c r="N8" s="2">
         <v>4101</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="14">
+        <v>4098</v>
+      </c>
+      <c r="P8" s="14">
+        <v>4101</v>
+      </c>
+      <c r="Q8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="R8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="3">
+      <c r="S8" s="15"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="3">
         <f t="shared" si="0"/>
-        <v>1.9559902200488996E-3</v>
-      </c>
-      <c r="S8" s="5">
+        <v>2.6894865525672372E-3</v>
+      </c>
+      <c r="V8" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="T8" s="3">
+      <c r="W8" s="3">
         <f t="shared" si="2"/>
-        <v>1.9559902200488996E-3</v>
-      </c>
-      <c r="U8" s="5">
+        <v>2.6894865525672372E-3</v>
+      </c>
+      <c r="X8" s="5">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
@@ -918,29 +1003,36 @@
       <c r="N9" s="2">
         <v>4139</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="14">
+        <v>4130</v>
+      </c>
+      <c r="P9" s="14">
+        <v>4135</v>
+      </c>
+      <c r="Q9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="3">
+      <c r="R9" s="7"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="3">
         <f t="shared" si="0"/>
-        <v>1.454192922927775E-3</v>
-      </c>
-      <c r="S9" s="5">
+        <v>3.1507513330101791E-3</v>
+      </c>
+      <c r="V9" s="5">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="T9" s="3">
+      <c r="W9" s="3">
         <f t="shared" si="2"/>
-        <v>1.454192922927775E-3</v>
-      </c>
-      <c r="U9" s="5">
+        <v>3.1507513330101791E-3</v>
+      </c>
+      <c r="X9" s="5">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
@@ -970,32 +1062,42 @@
       <c r="L10" s="10">
         <v>4165</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="14">
         <v>4166</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="N10" s="2">
+        <v>4180</v>
+      </c>
+      <c r="O10" s="14">
+        <v>4167</v>
+      </c>
+      <c r="P10" s="14">
+        <v>4180</v>
+      </c>
+      <c r="Q10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="3">
+      <c r="R10" s="7"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="3">
         <f t="shared" si="0"/>
-        <v>7.2063415805909202E-4</v>
-      </c>
-      <c r="S10" s="5">
+        <v>4.0835935623348548E-3</v>
+      </c>
+      <c r="V10" s="5">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="T10" s="3">
+      <c r="W10" s="3">
         <f t="shared" si="2"/>
-        <v>7.2063415805909202E-4</v>
-      </c>
-      <c r="U10" s="5">
+        <v>4.0835935623348548E-3</v>
+      </c>
+      <c r="X10" s="5">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1017,71 +1119,76 @@
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
-      <c r="O11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="5"/>
-    </row>
-    <row r="12" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="R11" s="7"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="5"/>
+    </row>
+    <row r="12" spans="3:30" x14ac:dyDescent="0.25">
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="7"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="5"/>
-    </row>
-    <row r="13" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="Q12" s="4"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="14"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="5"/>
+    </row>
+    <row r="13" spans="3:30" x14ac:dyDescent="0.25">
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="7"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="5"/>
-      <c r="X13" t="s">
+      <c r="Q13" s="4"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="14"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="5"/>
+      <c r="AA13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:30" x14ac:dyDescent="0.25">
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="7"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="5"/>
-      <c r="X14" t="s">
+      <c r="Q14" s="4"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="14"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="5"/>
+      <c r="AA14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:30" x14ac:dyDescent="0.25">
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="7"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="5"/>
-    </row>
-    <row r="16" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="Q15" s="4"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="14"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="5"/>
+    </row>
+    <row r="16" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="F16" s="1" t="s">
         <v>5</v>
@@ -1106,18 +1213,27 @@
       <c r="N16" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="O16" s="7" t="s">
+      <c r="O16" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="P16" s="7" t="s">
+      <c r="R16" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R16" s="3"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="5"/>
-    </row>
-    <row r="17" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="S16" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="U16" s="3"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="5"/>
+    </row>
+    <row r="17" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1156,33 +1272,40 @@
       <c r="N17" s="2">
         <v>576</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P17" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q17" s="2">
         <v>576</v>
       </c>
-      <c r="P17" s="7" t="s">
+      <c r="R17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="R17" s="3">
+      <c r="S17" s="14"/>
+      <c r="U17" s="3">
         <f>(N17-I17)/I17</f>
         <v>1.9469026548672566E-2</v>
       </c>
-      <c r="S17" s="5">
+      <c r="V17" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="T17" s="3">
+      <c r="W17" s="3">
         <f>(N17-J17)/J17</f>
         <v>0</v>
       </c>
-      <c r="U17" s="5">
+      <c r="X17" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AD17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
@@ -1218,30 +1341,34 @@
       <c r="N18" s="2">
         <v>597</v>
       </c>
-      <c r="O18" s="2">
+      <c r="P18" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q18" s="2">
         <v>597</v>
       </c>
-      <c r="P18" s="7" t="s">
+      <c r="R18" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="R18" s="3">
-        <f t="shared" ref="R18:R22" si="4">(N18-I18)/I18</f>
+      <c r="S18" s="14"/>
+      <c r="U18" s="3">
+        <f t="shared" ref="U18:U22" si="4">(N18-I18)/I18</f>
         <v>6.7453625632377737E-3</v>
       </c>
-      <c r="S18" s="5">
+      <c r="V18" s="5">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="T18" s="3">
-        <f t="shared" ref="T18:T21" si="5">(N18-J18)/J18</f>
+      <c r="W18" s="3">
+        <f t="shared" ref="W18:W21" si="5">(N18-J18)/J18</f>
         <v>1.6778523489932886E-3</v>
       </c>
-      <c r="U18" s="5">
+      <c r="X18" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1277,33 +1404,40 @@
       <c r="N19" s="12">
         <v>612</v>
       </c>
-      <c r="O19" s="2">
+      <c r="O19" s="14">
+        <v>608</v>
+      </c>
+      <c r="P19" s="14">
+        <v>612</v>
+      </c>
+      <c r="Q19" s="2">
         <v>617</v>
       </c>
-      <c r="P19" s="7" t="s">
+      <c r="R19" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R19" s="3">
+      <c r="S19" s="14"/>
+      <c r="U19" s="3">
         <f t="shared" si="4"/>
         <v>2.6845637583892617E-2</v>
       </c>
-      <c r="S19" s="5">
+      <c r="V19" s="5">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="T19" s="3">
+      <c r="W19" s="3">
         <f t="shared" si="5"/>
         <v>1.3245033112582781E-2</v>
       </c>
-      <c r="U19" s="5">
+      <c r="X19" s="5">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="AD19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
@@ -1339,31 +1473,38 @@
       <c r="N20" s="2">
         <v>635</v>
       </c>
-      <c r="O20" s="4" t="s">
+      <c r="O20" s="14">
+        <v>623</v>
+      </c>
+      <c r="P20" s="14">
+        <v>633</v>
+      </c>
+      <c r="Q20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P20" s="7"/>
-      <c r="R20" s="3">
+      <c r="R20" s="7"/>
+      <c r="S20" s="14"/>
+      <c r="U20" s="3">
         <f t="shared" si="4"/>
         <v>4.4407894736842105E-2</v>
       </c>
-      <c r="S20" s="5">
+      <c r="V20" s="5">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="T20" s="3">
+      <c r="W20" s="3">
         <f t="shared" si="5"/>
         <v>1.7628205128205128E-2</v>
       </c>
-      <c r="U20" s="5">
+      <c r="X20" s="5">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AA20" t="s">
+      <c r="AD20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1399,31 +1540,38 @@
       <c r="N21" s="2">
         <v>663</v>
       </c>
-      <c r="O21" s="4" t="s">
+      <c r="O21" s="14">
+        <v>646</v>
+      </c>
+      <c r="P21" s="14">
+        <v>659</v>
+      </c>
+      <c r="Q21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P21" s="7"/>
-      <c r="R21" s="3">
+      <c r="R21" s="7"/>
+      <c r="S21" s="14"/>
+      <c r="U21" s="3">
         <f t="shared" si="4"/>
         <v>3.110419906687403E-2</v>
       </c>
-      <c r="S21" s="5">
+      <c r="V21" s="5">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="T21" s="3">
+      <c r="W21" s="3">
         <f t="shared" si="5"/>
         <v>3.110419906687403E-2</v>
       </c>
-      <c r="U21" s="5">
+      <c r="X21" s="5">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="AA21" t="s">
+      <c r="AD21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1459,55 +1607,64 @@
       <c r="N22" s="2">
         <v>695</v>
       </c>
-      <c r="O22" s="4" t="s">
+      <c r="O22" s="14">
+        <v>665</v>
+      </c>
+      <c r="P22" s="14">
+        <v>679</v>
+      </c>
+      <c r="Q22" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P22" s="7"/>
-      <c r="R22" s="3">
+      <c r="R22" s="7"/>
+      <c r="S22" s="14"/>
+      <c r="U22" s="3">
         <f t="shared" si="4"/>
         <v>6.2691131498470942E-2</v>
       </c>
-      <c r="S22" s="5">
+      <c r="V22" s="5">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="T22" s="3">
+      <c r="W22" s="3">
         <f>(N22-J22)/J22</f>
         <v>6.2691131498470942E-2</v>
       </c>
-      <c r="U22" s="5">
+      <c r="X22" s="5">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AD22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:33" x14ac:dyDescent="0.25">
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="7"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="5"/>
-    </row>
-    <row r="24" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="Q23" s="4"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="14"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="5"/>
+    </row>
+    <row r="24" spans="3:33" x14ac:dyDescent="0.25">
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="7"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="5"/>
-    </row>
-    <row r="25" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="Q24" s="4"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="14"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="5"/>
+    </row>
+    <row r="25" spans="3:33" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="F25" s="1" t="s">
         <v>5</v>
@@ -1532,18 +1689,27 @@
       <c r="N25" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="O25" s="7" t="s">
+      <c r="O25" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="P25" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q25" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="P25" s="7" t="s">
+      <c r="R25" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R25" s="3"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="5"/>
-    </row>
-    <row r="26" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="S25" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="U25" s="3"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="5"/>
+    </row>
+    <row r="26" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>0</v>
       </c>
@@ -1579,33 +1745,36 @@
       <c r="M26" s="2">
         <v>2415</v>
       </c>
-      <c r="N26" s="14" t="s">
+      <c r="N26" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="O26" s="2">
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="2">
         <v>2415</v>
       </c>
-      <c r="P26" s="14" t="s">
+      <c r="R26" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="R26" s="3">
-        <f t="shared" si="0"/>
+      <c r="S26" s="14"/>
+      <c r="U26" s="3">
+        <f>(M26-I26)/I26</f>
         <v>9.8726114649681534E-2</v>
       </c>
-      <c r="S26" s="5">
+      <c r="V26" s="5">
         <f t="shared" si="1"/>
         <v>217</v>
       </c>
-      <c r="T26" s="3">
-        <f t="shared" si="2"/>
+      <c r="W26" s="3">
+        <f>(M26-J26)/J26</f>
         <v>0</v>
       </c>
-      <c r="U26" s="5">
+      <c r="X26" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>1</v>
       </c>
@@ -1638,35 +1807,38 @@
       <c r="M27" s="2">
         <v>2614</v>
       </c>
-      <c r="N27" s="14"/>
-      <c r="O27" s="4" t="s">
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P27" s="14"/>
-      <c r="R27" s="3">
-        <f t="shared" si="0"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="14"/>
+      <c r="U27" s="3">
+        <f>(M27-I27)/I27</f>
         <v>2.7111984282907661E-2</v>
       </c>
-      <c r="S27" s="5">
+      <c r="V27" s="5">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="T27" s="3">
-        <f t="shared" si="2"/>
+      <c r="W27" s="3">
+        <f>(M27-J27)/J27</f>
         <v>2.7111984282907661E-2</v>
       </c>
-      <c r="U27" s="5">
+      <c r="X27" s="5">
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="3"/>
-      <c r="Z27" s="3"/>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="5"/>
-      <c r="AD27" s="5"/>
-    </row>
-    <row r="28" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="5"/>
+      <c r="AG27" s="5"/>
+    </row>
+    <row r="28" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
@@ -1699,35 +1871,38 @@
       <c r="M28" s="2">
         <v>2660</v>
       </c>
-      <c r="N28" s="14"/>
-      <c r="O28" s="4" t="s">
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P28" s="14"/>
-      <c r="R28" s="3">
-        <f t="shared" si="0"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="14"/>
+      <c r="U28" s="3">
+        <f>(M28-I28)/I28</f>
         <v>1.0638297872340425E-2</v>
       </c>
-      <c r="S28" s="5">
+      <c r="V28" s="5">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="T28" s="3">
-        <f t="shared" si="2"/>
+      <c r="W28" s="3">
+        <f>(M28-J28)/J28</f>
         <v>7.9575596816976128E-3</v>
       </c>
-      <c r="U28" s="5">
+      <c r="X28" s="5">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="3"/>
-      <c r="Z28" s="3"/>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="5"/>
-      <c r="AD28" s="5"/>
-    </row>
-    <row r="29" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="5"/>
+      <c r="AG28" s="5"/>
+    </row>
+    <row r="29" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
@@ -1760,35 +1935,38 @@
       <c r="M29" s="2">
         <v>2734</v>
       </c>
-      <c r="N29" s="14"/>
-      <c r="O29" s="4" t="s">
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P29" s="14"/>
-      <c r="R29" s="3">
-        <f t="shared" si="0"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="14"/>
+      <c r="U29" s="3">
+        <f>(M29-I29)/I29</f>
         <v>9.9741411156261551E-3</v>
       </c>
-      <c r="S29" s="5">
+      <c r="V29" s="5">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="T29" s="3">
-        <f t="shared" si="2"/>
+      <c r="W29" s="3">
+        <f>(M29-J29)/J29</f>
         <v>9.9741411156261551E-3</v>
       </c>
-      <c r="U29" s="5">
+      <c r="X29" s="5">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="3"/>
-      <c r="Z29" s="3"/>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="5"/>
-      <c r="AD29" s="5"/>
-    </row>
-    <row r="30" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="5"/>
+      <c r="AG29" s="5"/>
+    </row>
+    <row r="30" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
@@ -1821,35 +1999,38 @@
       <c r="M30" s="2">
         <v>2836</v>
       </c>
-      <c r="N30" s="14"/>
-      <c r="O30" s="4" t="s">
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P30" s="14"/>
-      <c r="R30" s="3">
-        <f t="shared" si="0"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="14"/>
+      <c r="U30" s="3">
+        <f>(M30-I30)/I30</f>
         <v>1.9410496046010063E-2</v>
       </c>
-      <c r="S30" s="5">
+      <c r="V30" s="5">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="T30" s="3">
-        <f t="shared" si="2"/>
+      <c r="W30" s="3">
+        <f>(M30-J30)/J30</f>
         <v>1.9410496046010063E-2</v>
       </c>
-      <c r="U30" s="5">
+      <c r="X30" s="5">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
-      <c r="X30" s="1"/>
-      <c r="Y30" s="3"/>
-      <c r="Z30" s="3"/>
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="5"/>
-      <c r="AD30" s="5"/>
-    </row>
-    <row r="31" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AE30" s="1"/>
+      <c r="AF30" s="5"/>
+      <c r="AG30" s="5"/>
+    </row>
+    <row r="31" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
@@ -1871,59 +2052,64 @@
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="4" t="s">
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P31" s="14"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="5"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="3"/>
-      <c r="Z31" s="3"/>
-      <c r="AB31" s="1"/>
-      <c r="AC31" s="5"/>
-      <c r="AD31" s="5"/>
-    </row>
-    <row r="32" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="R31" s="15"/>
+      <c r="S31" s="14"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="5"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AE31" s="1"/>
+      <c r="AF31" s="5"/>
+      <c r="AG31" s="5"/>
+    </row>
+    <row r="32" spans="3:33" x14ac:dyDescent="0.25">
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="7"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="5"/>
-      <c r="X32" s="1"/>
-      <c r="Y32" s="3"/>
-      <c r="Z32" s="3"/>
-      <c r="AB32" s="1"/>
-      <c r="AC32" s="5"/>
-      <c r="AD32" s="5"/>
-    </row>
-    <row r="33" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="Q32" s="4"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="14"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="5"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AE32" s="1"/>
+      <c r="AF32" s="5"/>
+      <c r="AG32" s="5"/>
+    </row>
+    <row r="33" spans="3:33" x14ac:dyDescent="0.25">
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="7"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="3"/>
-      <c r="U33" s="5"/>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="3"/>
-      <c r="Z33" s="3"/>
-      <c r="AB33" s="1"/>
-      <c r="AC33" s="5"/>
-      <c r="AD33" s="5"/>
-    </row>
-    <row r="34" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="Q33" s="4"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="14"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="5"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AE33" s="1"/>
+      <c r="AF33" s="5"/>
+      <c r="AG33" s="5"/>
+    </row>
+    <row r="34" spans="3:33" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="F34" s="1" t="s">
         <v>5</v>
@@ -1948,24 +2134,33 @@
       <c r="N34" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="O34" s="7" t="s">
+      <c r="O34" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="P34" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q34" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="P34" s="7" t="s">
+      <c r="R34" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R34" s="3"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="3"/>
-      <c r="U34" s="5"/>
-      <c r="X34" s="1"/>
-      <c r="Y34" s="3"/>
-      <c r="Z34" s="3"/>
-      <c r="AB34" s="1"/>
-      <c r="AC34" s="5"/>
-      <c r="AD34" s="5"/>
-    </row>
-    <row r="35" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="S34" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="U34" s="3"/>
+      <c r="V34" s="5"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="5"/>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3"/>
+      <c r="AE34" s="1"/>
+      <c r="AF34" s="5"/>
+      <c r="AG34" s="5"/>
+    </row>
+    <row r="35" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>0</v>
       </c>
@@ -2004,36 +2199,43 @@
       <c r="N35" s="2">
         <v>705</v>
       </c>
-      <c r="O35" s="2">
+      <c r="O35" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P35" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q35" s="2">
         <v>705</v>
       </c>
-      <c r="P35" s="7" t="s">
+      <c r="R35" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="R35" s="3">
-        <f t="shared" si="0"/>
+      <c r="S35" s="14"/>
+      <c r="U35" s="3">
+        <f>(N35-I35)/I35</f>
         <v>4.2899408284023666E-2</v>
       </c>
-      <c r="S35" s="5">
+      <c r="V35" s="5">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="T35" s="3">
-        <f t="shared" si="2"/>
+      <c r="W35" s="3">
+        <f>(N35-J35)/J35</f>
         <v>0</v>
       </c>
-      <c r="U35" s="5">
+      <c r="X35" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X35" s="1"/>
-      <c r="Y35" s="3"/>
-      <c r="Z35" s="3"/>
-      <c r="AB35" s="1"/>
-      <c r="AC35" s="5"/>
-      <c r="AD35" s="5"/>
-    </row>
-    <row r="36" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="3"/>
+      <c r="AC35" s="3"/>
+      <c r="AE35" s="1"/>
+      <c r="AF35" s="5"/>
+      <c r="AG35" s="5"/>
+    </row>
+    <row r="36" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>1</v>
       </c>
@@ -2069,36 +2271,40 @@
       <c r="N36" s="2">
         <v>768</v>
       </c>
-      <c r="O36" s="2">
+      <c r="P36" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q36" s="2">
         <v>768</v>
       </c>
-      <c r="P36" s="7" t="s">
+      <c r="R36" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="R36" s="3">
-        <f t="shared" si="0"/>
-        <v>2.6631158455392811E-3</v>
-      </c>
-      <c r="S36" s="5">
+      <c r="S36" s="14"/>
+      <c r="U36" s="3">
+        <f t="shared" ref="U36:U40" si="6">(N36-I36)/I36</f>
+        <v>2.2636484687083888E-2</v>
+      </c>
+      <c r="V36" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="T36" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U36" s="5">
+      <c r="W36" s="3">
+        <f t="shared" ref="W36:W40" si="7">(N36-J36)/J36</f>
+        <v>1.9920318725099601E-2</v>
+      </c>
+      <c r="X36" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X36" s="1"/>
-      <c r="Y36" s="3"/>
-      <c r="Z36" s="3"/>
-      <c r="AB36" s="1"/>
-      <c r="AC36" s="5"/>
-      <c r="AD36" s="5"/>
-    </row>
-    <row r="37" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="3"/>
+      <c r="AE36" s="1"/>
+      <c r="AF36" s="5"/>
+      <c r="AG36" s="5"/>
+    </row>
+    <row r="37" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>2</v>
       </c>
@@ -2128,39 +2334,49 @@
       <c r="L37" s="10">
         <v>783</v>
       </c>
-      <c r="M37" s="2">
+      <c r="M37" s="14">
         <v>787</v>
       </c>
-      <c r="O37" s="4" t="s">
+      <c r="N37" s="2">
+        <v>796</v>
+      </c>
+      <c r="O37" s="14">
+        <v>776</v>
+      </c>
+      <c r="P37" s="14">
+        <v>794</v>
+      </c>
+      <c r="Q37" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P37" s="7" t="s">
+      <c r="R37" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="R37" s="3">
-        <f t="shared" si="0"/>
-        <v>2.2077922077922078E-2</v>
-      </c>
-      <c r="S37" s="5">
+      <c r="S37" s="14"/>
+      <c r="U37" s="3">
+        <f t="shared" si="6"/>
+        <v>3.3766233766233764E-2</v>
+      </c>
+      <c r="V37" s="5">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="T37" s="3">
-        <f t="shared" si="2"/>
-        <v>1.0269576379974325E-2</v>
-      </c>
-      <c r="U37" s="5">
+      <c r="W37" s="3">
+        <f t="shared" si="7"/>
+        <v>2.1822849807445442E-2</v>
+      </c>
+      <c r="X37" s="5">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="X37" s="1"/>
-      <c r="Y37" s="3"/>
-      <c r="Z37" s="3"/>
-      <c r="AB37" s="1"/>
-      <c r="AC37" s="5"/>
-      <c r="AD37" s="5"/>
-    </row>
-    <row r="38" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="3"/>
+      <c r="AC37" s="3"/>
+      <c r="AE37" s="1"/>
+      <c r="AF37" s="5"/>
+      <c r="AG37" s="5"/>
+    </row>
+    <row r="38" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
@@ -2184,43 +2400,53 @@
       <c r="J38" s="9">
         <v>809</v>
       </c>
-      <c r="K38" s="9">
-        <v>816</v>
+      <c r="K38" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="L38" s="10">
-        <v>816</v>
-      </c>
-      <c r="M38" s="2">
+        <v>817</v>
+      </c>
+      <c r="M38" s="14">
         <v>819</v>
       </c>
-      <c r="O38" s="4" t="s">
+      <c r="N38" s="2">
+        <v>826</v>
+      </c>
+      <c r="O38" s="14">
+        <v>812</v>
+      </c>
+      <c r="P38" s="14">
+        <v>823</v>
+      </c>
+      <c r="Q38" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P38" s="7"/>
-      <c r="R38" s="3">
-        <f t="shared" si="0"/>
-        <v>1.3613861386138614E-2</v>
-      </c>
-      <c r="S38" s="5">
+      <c r="R38" s="7"/>
+      <c r="S38" s="14"/>
+      <c r="U38" s="3">
+        <f t="shared" si="6"/>
+        <v>2.2277227722772276E-2</v>
+      </c>
+      <c r="V38" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="T38" s="3">
-        <f t="shared" si="2"/>
-        <v>1.2360939431396786E-2</v>
-      </c>
-      <c r="U38" s="5">
+      <c r="W38" s="3">
+        <f t="shared" si="7"/>
+        <v>2.1013597033374538E-2</v>
+      </c>
+      <c r="X38" s="5">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="3"/>
-      <c r="Z38" s="3"/>
-      <c r="AB38" s="1"/>
-      <c r="AC38" s="5"/>
-      <c r="AD38" s="5"/>
-    </row>
-    <row r="39" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="3"/>
+      <c r="AC38" s="3"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="5"/>
+      <c r="AG38" s="5"/>
+    </row>
+    <row r="39" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>16</v>
       </c>
@@ -2244,43 +2470,53 @@
       <c r="J39" s="9">
         <v>826</v>
       </c>
-      <c r="K39" s="9">
-        <v>843</v>
+      <c r="K39" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="L39" s="10">
         <v>843</v>
       </c>
-      <c r="M39" s="2">
+      <c r="M39" s="14">
         <v>845</v>
       </c>
-      <c r="O39" s="4" t="s">
+      <c r="N39" s="2">
+        <v>871</v>
+      </c>
+      <c r="O39" s="14">
+        <v>842</v>
+      </c>
+      <c r="P39" s="14">
+        <v>865</v>
+      </c>
+      <c r="Q39" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P39" s="7"/>
-      <c r="R39" s="3">
-        <f t="shared" si="0"/>
-        <v>2.3002421307506054E-2</v>
-      </c>
-      <c r="S39" s="5">
+      <c r="R39" s="7"/>
+      <c r="S39" s="14"/>
+      <c r="U39" s="3">
+        <f t="shared" si="6"/>
+        <v>5.4479418886198547E-2</v>
+      </c>
+      <c r="V39" s="5">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="T39" s="3">
-        <f t="shared" si="2"/>
-        <v>2.3002421307506054E-2</v>
-      </c>
-      <c r="U39" s="5">
+      <c r="W39" s="3">
+        <f t="shared" si="7"/>
+        <v>5.4479418886198547E-2</v>
+      </c>
+      <c r="X39" s="5">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="X39" s="1"/>
-      <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
-      <c r="AB39" s="1"/>
-      <c r="AC39" s="5"/>
-      <c r="AD39" s="5"/>
-    </row>
-    <row r="40" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA39" s="1"/>
+      <c r="AB39" s="3"/>
+      <c r="AC39" s="3"/>
+      <c r="AE39" s="1"/>
+      <c r="AF39" s="5"/>
+      <c r="AG39" s="5"/>
+    </row>
+    <row r="40" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>4</v>
       </c>
@@ -2310,73 +2546,86 @@
       <c r="L40" s="10">
         <v>864</v>
       </c>
-      <c r="M40" s="2">
+      <c r="M40" s="14">
         <v>871</v>
       </c>
-      <c r="O40" s="4" t="s">
+      <c r="N40" s="2">
+        <v>911</v>
+      </c>
+      <c r="O40" s="14">
+        <v>868</v>
+      </c>
+      <c r="P40" s="14">
+        <v>909</v>
+      </c>
+      <c r="Q40" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P40" s="7"/>
-      <c r="R40" s="3">
-        <f t="shared" si="0"/>
-        <v>1.1614401858304297E-2</v>
-      </c>
-      <c r="S40" s="5">
+      <c r="R40" s="7"/>
+      <c r="S40" s="14"/>
+      <c r="U40" s="3">
+        <f t="shared" si="6"/>
+        <v>5.8072009291521488E-2</v>
+      </c>
+      <c r="V40" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="T40" s="3">
-        <f t="shared" si="2"/>
-        <v>1.1614401858304297E-2</v>
-      </c>
-      <c r="U40" s="5">
+      <c r="W40" s="3">
+        <f t="shared" si="7"/>
+        <v>5.8072009291521488E-2</v>
+      </c>
+      <c r="X40" s="5">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="X40" s="1"/>
-      <c r="Y40" s="3"/>
-      <c r="Z40" s="3"/>
-      <c r="AB40" s="1"/>
-      <c r="AC40" s="5"/>
-      <c r="AD40" s="5"/>
-    </row>
-    <row r="41" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA40" s="1"/>
+      <c r="AB40" s="3"/>
+      <c r="AC40" s="3"/>
+      <c r="AE40" s="1"/>
+      <c r="AF40" s="5"/>
+      <c r="AG40" s="5"/>
+    </row>
+    <row r="41" spans="3:33" x14ac:dyDescent="0.25">
       <c r="I41" s="11"/>
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
       <c r="L41" s="11"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="7"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="5"/>
-      <c r="X41" s="1"/>
-      <c r="Y41" s="3"/>
-      <c r="Z41" s="3"/>
-      <c r="AB41" s="1"/>
-      <c r="AC41" s="5"/>
-      <c r="AD41" s="5"/>
-    </row>
-    <row r="42" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="M41" s="16"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="14"/>
+      <c r="U41" s="3"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="3"/>
+      <c r="X41" s="5"/>
+      <c r="AA41" s="1"/>
+      <c r="AB41" s="3"/>
+      <c r="AC41" s="3"/>
+      <c r="AE41" s="1"/>
+      <c r="AF41" s="5"/>
+      <c r="AG41" s="5"/>
+    </row>
+    <row r="42" spans="3:33" x14ac:dyDescent="0.25">
       <c r="I42" s="11"/>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
       <c r="L42" s="11"/>
-      <c r="O42" s="4"/>
-      <c r="P42" s="7"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="5"/>
-      <c r="X42" s="1"/>
-      <c r="Y42" s="3"/>
-      <c r="Z42" s="3"/>
-      <c r="AB42" s="1"/>
-      <c r="AC42" s="5"/>
-      <c r="AD42" s="5"/>
-    </row>
-    <row r="43" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="Q42" s="4"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="14"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="5"/>
+      <c r="AA42" s="1"/>
+      <c r="AB42" s="3"/>
+      <c r="AC42" s="3"/>
+      <c r="AE42" s="1"/>
+      <c r="AF42" s="5"/>
+      <c r="AG42" s="5"/>
+    </row>
+    <row r="43" spans="3:33" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
       <c r="F43" s="1" t="s">
         <v>5</v>
@@ -2401,24 +2650,33 @@
       <c r="N43" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="O43" s="7" t="s">
+      <c r="O43" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="P43" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q43" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="P43" s="7" t="s">
+      <c r="R43" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R43" s="3"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="3"/>
-      <c r="U43" s="5"/>
-      <c r="X43" s="1"/>
-      <c r="Y43" s="3"/>
-      <c r="Z43" s="3"/>
-      <c r="AB43" s="1"/>
-      <c r="AC43" s="5"/>
-      <c r="AD43" s="5"/>
-    </row>
-    <row r="44" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="S43" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="U43" s="3"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="5"/>
+      <c r="AA43" s="1"/>
+      <c r="AB43" s="3"/>
+      <c r="AC43" s="3"/>
+      <c r="AE43" s="1"/>
+      <c r="AF43" s="5"/>
+      <c r="AG43" s="5"/>
+    </row>
+    <row r="44" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>0</v>
       </c>
@@ -2454,36 +2712,43 @@
       <c r="N44" s="2">
         <v>14032</v>
       </c>
-      <c r="O44" s="2">
+      <c r="O44" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P44" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q44" s="2">
         <v>14032</v>
       </c>
-      <c r="P44" s="7" t="s">
+      <c r="R44" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="R44" s="3">
-        <f t="shared" ref="R44:R46" si="6">(M44-I44)/I44</f>
+      <c r="S44" s="14"/>
+      <c r="U44" s="3">
+        <f t="shared" ref="U44:U46" si="8">(M44-I44)/I44</f>
         <v>5.8060354096480535E-3</v>
       </c>
-      <c r="S44" s="5">
-        <f t="shared" ref="S44:S46" si="7">M44-I44</f>
+      <c r="V44" s="5">
+        <f t="shared" ref="V44:V46" si="9">M44-I44</f>
         <v>81</v>
       </c>
-      <c r="T44" s="3">
-        <f t="shared" ref="T44:T46" si="8">(M44-J44)/J44</f>
+      <c r="W44" s="3">
+        <f t="shared" ref="W44:W46" si="10">(M44-J44)/J44</f>
         <v>5.8060354096480535E-3</v>
       </c>
-      <c r="U44" s="5">
-        <f t="shared" ref="U44:U46" si="9">M44-J44</f>
+      <c r="X44" s="5">
+        <f t="shared" ref="X44:X46" si="11">M44-J44</f>
         <v>81</v>
       </c>
-      <c r="X44" s="1"/>
-      <c r="Y44" s="3"/>
-      <c r="Z44" s="3"/>
-      <c r="AB44" s="1"/>
-      <c r="AC44" s="5"/>
-      <c r="AD44" s="5"/>
-    </row>
-    <row r="45" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA44" s="1"/>
+      <c r="AB44" s="3"/>
+      <c r="AC44" s="3"/>
+      <c r="AE44" s="1"/>
+      <c r="AF44" s="5"/>
+      <c r="AG44" s="5"/>
+    </row>
+    <row r="45" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>1</v>
       </c>
@@ -2516,39 +2781,45 @@
       <c r="M45" s="8">
         <v>15233</v>
       </c>
-      <c r="N45" s="2">
+      <c r="N45" s="17">
         <v>15274</v>
       </c>
-      <c r="O45" s="2">
+      <c r="P45" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q45" s="2">
         <v>15274</v>
       </c>
-      <c r="P45" s="7" t="s">
+      <c r="R45" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="R45" s="3">
-        <f t="shared" si="6"/>
-        <v>1.384359400998336E-2</v>
-      </c>
-      <c r="S45" s="5">
-        <f t="shared" si="7"/>
-        <v>208</v>
-      </c>
-      <c r="T45" s="3">
+      <c r="S45" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="U45" s="3">
         <f t="shared" si="8"/>
         <v>1.384359400998336E-2</v>
       </c>
-      <c r="U45" s="5">
+      <c r="V45" s="5">
         <f t="shared" si="9"/>
         <v>208</v>
       </c>
-      <c r="X45" s="1"/>
-      <c r="Y45" s="3"/>
-      <c r="Z45" s="3"/>
-      <c r="AB45" s="1"/>
-      <c r="AC45" s="5"/>
-      <c r="AD45" s="5"/>
-    </row>
-    <row r="46" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="W45" s="3">
+        <f t="shared" si="10"/>
+        <v>1.384359400998336E-2</v>
+      </c>
+      <c r="X45" s="5">
+        <f t="shared" si="11"/>
+        <v>208</v>
+      </c>
+      <c r="AA45" s="1"/>
+      <c r="AB45" s="3"/>
+      <c r="AC45" s="3"/>
+      <c r="AE45" s="1"/>
+      <c r="AF45" s="5"/>
+      <c r="AG45" s="5"/>
+    </row>
+    <row r="46" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>2</v>
       </c>
@@ -2581,34 +2852,43 @@
       <c r="M46" s="2">
         <v>15376</v>
       </c>
-      <c r="O46" s="4" t="s">
+      <c r="N46" s="17">
+        <v>15765</v>
+      </c>
+      <c r="O46" s="14">
+        <v>15365</v>
+      </c>
+      <c r="Q46" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P46" s="7"/>
-      <c r="R46" s="3">
-        <f t="shared" si="6"/>
-        <v>1.8278145695364238E-2</v>
-      </c>
-      <c r="S46" s="5">
-        <f t="shared" si="7"/>
-        <v>276</v>
-      </c>
-      <c r="T46" s="3">
+      <c r="R46" s="7"/>
+      <c r="S46" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="U46" s="3">
         <f t="shared" si="8"/>
         <v>1.8278145695364238E-2</v>
       </c>
-      <c r="U46" s="5">
+      <c r="V46" s="5">
         <f t="shared" si="9"/>
         <v>276</v>
       </c>
-      <c r="X46" s="1"/>
-      <c r="Y46" s="3"/>
-      <c r="Z46" s="3"/>
-      <c r="AB46" s="1"/>
-      <c r="AC46" s="5"/>
-      <c r="AD46" s="5"/>
-    </row>
-    <row r="47" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="W46" s="3">
+        <f t="shared" si="10"/>
+        <v>1.8278145695364238E-2</v>
+      </c>
+      <c r="X46" s="5">
+        <f t="shared" si="11"/>
+        <v>276</v>
+      </c>
+      <c r="AA46" s="1"/>
+      <c r="AB46" s="3"/>
+      <c r="AC46" s="3"/>
+      <c r="AE46" s="1"/>
+      <c r="AF46" s="5"/>
+      <c r="AG46" s="5"/>
+    </row>
+    <row r="47" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
         <v>3</v>
       </c>
@@ -2641,34 +2921,38 @@
       <c r="M47" s="2">
         <v>15737</v>
       </c>
-      <c r="O47" s="4" t="s">
+      <c r="O47" s="14">
+        <v>15737</v>
+      </c>
+      <c r="Q47" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P47" s="7"/>
-      <c r="R47" s="3">
-        <f t="shared" ref="R47" si="10">(M47-I47)/I47</f>
+      <c r="R47" s="7"/>
+      <c r="S47" s="14"/>
+      <c r="U47" s="3">
+        <f t="shared" ref="U47" si="12">(M47-I47)/I47</f>
         <v>3.443218771918638E-3</v>
       </c>
-      <c r="S47" s="5">
-        <f t="shared" ref="S47" si="11">M47-I47</f>
+      <c r="V47" s="5">
+        <f t="shared" ref="V47" si="13">M47-I47</f>
         <v>54</v>
       </c>
-      <c r="T47" s="3">
-        <f t="shared" ref="T47" si="12">(M47-J47)/J47</f>
+      <c r="W47" s="3">
+        <f t="shared" ref="W47" si="14">(M47-J47)/J47</f>
         <v>3.443218771918638E-3</v>
       </c>
-      <c r="U47" s="5">
-        <f t="shared" ref="U47" si="13">M47-J47</f>
+      <c r="X47" s="5">
+        <f t="shared" ref="X47" si="15">M47-J47</f>
         <v>54</v>
       </c>
-      <c r="X47" s="1"/>
-      <c r="Y47" s="3"/>
-      <c r="Z47" s="3"/>
-      <c r="AB47" s="1"/>
-      <c r="AC47" s="5"/>
-      <c r="AD47" s="5"/>
-    </row>
-    <row r="48" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA47" s="1"/>
+      <c r="AB47" s="3"/>
+      <c r="AC47" s="3"/>
+      <c r="AE47" s="1"/>
+      <c r="AF47" s="5"/>
+      <c r="AG47" s="5"/>
+    </row>
+    <row r="48" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
         <v>16</v>
       </c>
@@ -2690,22 +2974,26 @@
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
-      <c r="O48" s="4" t="s">
+      <c r="O48" s="14">
+        <v>15999</v>
+      </c>
+      <c r="Q48" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P48" s="7"/>
-      <c r="R48" s="3"/>
-      <c r="S48" s="5"/>
-      <c r="T48" s="3"/>
-      <c r="U48" s="5"/>
-      <c r="X48" s="1"/>
-      <c r="Y48" s="3"/>
-      <c r="Z48" s="3"/>
-      <c r="AB48" s="1"/>
-      <c r="AC48" s="5"/>
-      <c r="AD48" s="5"/>
-    </row>
-    <row r="49" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="R48" s="7"/>
+      <c r="S48" s="14"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="3"/>
+      <c r="X48" s="5"/>
+      <c r="AA48" s="1"/>
+      <c r="AB48" s="3"/>
+      <c r="AC48" s="3"/>
+      <c r="AE48" s="1"/>
+      <c r="AF48" s="5"/>
+      <c r="AG48" s="5"/>
+    </row>
+    <row r="49" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
@@ -2723,252 +3011,264 @@
         <f>POWER(2,F49)*D45</f>
         <v>1217280</v>
       </c>
-      <c r="I49" s="1"/>
+      <c r="I49" s="1">
+        <v>16227</v>
+      </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
-      <c r="O49" s="4" t="s">
+      <c r="O49" s="14">
+        <v>16296</v>
+      </c>
+      <c r="P49" s="17">
+        <v>16415</v>
+      </c>
+      <c r="Q49" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P49" s="7"/>
-      <c r="R49" s="3"/>
-      <c r="S49" s="3"/>
-      <c r="T49" s="3"/>
+      <c r="R49" s="7"/>
+      <c r="S49" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="U49" s="3"/>
-      <c r="X49" s="1"/>
-      <c r="Y49" s="3"/>
-      <c r="Z49" s="3"/>
-      <c r="AB49" s="1"/>
-      <c r="AC49" s="5"/>
-      <c r="AD49" s="5"/>
-    </row>
-    <row r="50" spans="3:30" x14ac:dyDescent="0.25">
-      <c r="X50" s="1"/>
-      <c r="Y50" s="3"/>
-      <c r="Z50" s="3"/>
-      <c r="AB50" s="1"/>
-      <c r="AC50" s="5"/>
-      <c r="AD50" s="5"/>
-    </row>
-    <row r="51" spans="3:30" x14ac:dyDescent="0.25">
-      <c r="X51" s="1"/>
-      <c r="Y51" s="3"/>
-      <c r="Z51" s="3"/>
-      <c r="AB51" s="1"/>
-      <c r="AC51" s="5"/>
-      <c r="AD51" s="5"/>
-    </row>
-    <row r="52" spans="3:30" x14ac:dyDescent="0.25">
-      <c r="AB52" s="1"/>
-      <c r="AC52" s="3"/>
-      <c r="AD52" s="3"/>
-    </row>
-    <row r="60" spans="3:30" x14ac:dyDescent="0.25">
-      <c r="X60" s="1"/>
-      <c r="Y60" s="3"/>
-      <c r="Z60" s="3"/>
-      <c r="AB60" s="1"/>
-      <c r="AC60" s="5"/>
-      <c r="AD60" s="5"/>
-    </row>
-    <row r="61" spans="3:30" x14ac:dyDescent="0.25">
-      <c r="X61" s="1"/>
-      <c r="Y61" s="3"/>
-      <c r="Z61" s="3"/>
-      <c r="AB61" s="1"/>
-      <c r="AC61" s="5"/>
-      <c r="AD61" s="5"/>
-    </row>
-    <row r="62" spans="3:30" x14ac:dyDescent="0.25">
-      <c r="X62" s="1"/>
-      <c r="Y62" s="3"/>
-      <c r="Z62" s="3"/>
-      <c r="AB62" s="1"/>
-      <c r="AC62" s="5"/>
-      <c r="AD62" s="5"/>
-    </row>
-    <row r="63" spans="3:30" x14ac:dyDescent="0.25">
-      <c r="X63" s="1"/>
-      <c r="Y63" s="3"/>
-      <c r="Z63" s="3"/>
-      <c r="AB63" s="1"/>
-      <c r="AC63" s="5"/>
-      <c r="AD63" s="5"/>
-    </row>
-    <row r="64" spans="3:30" x14ac:dyDescent="0.25">
-      <c r="X64" s="1"/>
-      <c r="Y64" s="3"/>
-      <c r="Z64" s="3"/>
-      <c r="AB64" s="1"/>
-      <c r="AC64" s="5"/>
-      <c r="AD64" s="5"/>
-    </row>
-    <row r="65" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X65" s="1"/>
-      <c r="Y65" s="3"/>
-      <c r="Z65" s="3"/>
-      <c r="AB65" s="1"/>
-      <c r="AC65" s="5"/>
-      <c r="AD65" s="5"/>
-    </row>
-    <row r="66" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X66" s="1"/>
-      <c r="Y66" s="3"/>
-      <c r="Z66" s="3"/>
-      <c r="AB66" s="1"/>
-      <c r="AC66" s="5"/>
-      <c r="AD66" s="5"/>
-    </row>
-    <row r="67" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X67" s="1"/>
-      <c r="Y67" s="3"/>
-      <c r="Z67" s="3"/>
-      <c r="AB67" s="1"/>
-      <c r="AC67" s="5"/>
-      <c r="AD67" s="5"/>
-    </row>
-    <row r="68" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X68" s="1"/>
-      <c r="Y68" s="3"/>
-      <c r="Z68" s="3"/>
-      <c r="AB68" s="1"/>
-      <c r="AC68" s="5"/>
-      <c r="AD68" s="5"/>
-    </row>
-    <row r="69" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X69" s="1"/>
-      <c r="Y69" s="3"/>
-      <c r="Z69" s="3"/>
-      <c r="AB69" s="1"/>
-      <c r="AC69" s="5"/>
-      <c r="AD69" s="5"/>
-    </row>
-    <row r="70" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X70" s="1"/>
-      <c r="Y70" s="3"/>
-      <c r="Z70" s="3"/>
-      <c r="AB70" s="1"/>
-      <c r="AC70" s="5"/>
-      <c r="AD70" s="5"/>
-    </row>
-    <row r="71" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X71" s="1"/>
-      <c r="Y71" s="3"/>
-      <c r="Z71" s="3"/>
-      <c r="AB71" s="1"/>
-      <c r="AC71" s="5"/>
-      <c r="AD71" s="5"/>
-    </row>
-    <row r="72" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X72" s="1"/>
-      <c r="Y72" s="3"/>
-      <c r="Z72" s="3"/>
-      <c r="AB72" s="1"/>
-      <c r="AC72" s="5"/>
-      <c r="AD72" s="5"/>
-    </row>
-    <row r="73" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X73" s="1"/>
-      <c r="Y73" s="3"/>
-      <c r="Z73" s="3"/>
-      <c r="AB73" s="1"/>
-      <c r="AC73" s="5"/>
-      <c r="AD73" s="5"/>
-    </row>
-    <row r="74" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X74" s="1"/>
-      <c r="Y74" s="3"/>
-      <c r="Z74" s="3"/>
-      <c r="AB74" s="1"/>
-      <c r="AC74" s="5"/>
-      <c r="AD74" s="5"/>
-    </row>
-    <row r="75" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X75" s="1"/>
-      <c r="Y75" s="3"/>
-      <c r="Z75" s="3"/>
-      <c r="AB75" s="1"/>
-      <c r="AC75" s="5"/>
-      <c r="AD75" s="5"/>
-    </row>
-    <row r="76" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X76" s="1"/>
-      <c r="Y76" s="3"/>
-      <c r="Z76" s="3"/>
-      <c r="AB76" s="1"/>
-      <c r="AC76" s="5"/>
-      <c r="AD76" s="5"/>
-    </row>
-    <row r="77" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X77" s="1"/>
-      <c r="Y77" s="3"/>
-      <c r="Z77" s="3"/>
-      <c r="AB77" s="1"/>
-      <c r="AC77" s="5"/>
-      <c r="AD77" s="5"/>
-    </row>
-    <row r="78" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X78" s="1"/>
-      <c r="Y78" s="3"/>
-      <c r="Z78" s="3"/>
-      <c r="AB78" s="1"/>
-      <c r="AC78" s="5"/>
-      <c r="AD78" s="5"/>
-    </row>
-    <row r="79" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X79" s="1"/>
-      <c r="Y79" s="3"/>
-      <c r="Z79" s="3"/>
-      <c r="AB79" s="1"/>
-      <c r="AC79" s="5"/>
-      <c r="AD79" s="5"/>
-    </row>
-    <row r="80" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X80" s="1"/>
-      <c r="Y80" s="3"/>
-      <c r="Z80" s="3"/>
-      <c r="AB80" s="1"/>
-      <c r="AC80" s="5"/>
-      <c r="AD80" s="5"/>
-    </row>
-    <row r="81" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X81" s="1"/>
-      <c r="Y81" s="3"/>
-      <c r="Z81" s="3"/>
-      <c r="AB81" s="1"/>
-      <c r="AC81" s="5"/>
-      <c r="AD81" s="5"/>
-    </row>
-    <row r="82" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X82" s="1"/>
-      <c r="Y82" s="3"/>
-      <c r="Z82" s="3"/>
-      <c r="AB82" s="1"/>
-      <c r="AC82" s="5"/>
-      <c r="AD82" s="5"/>
-    </row>
-    <row r="83" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X83" s="1"/>
-      <c r="Y83" s="3"/>
-      <c r="Z83" s="3"/>
-      <c r="AB83" s="1"/>
-      <c r="AC83" s="5"/>
-      <c r="AD83" s="5"/>
-    </row>
-    <row r="84" spans="24:30" x14ac:dyDescent="0.25">
-      <c r="X84" s="1"/>
-      <c r="Y84" s="3"/>
-      <c r="Z84" s="3"/>
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
+      <c r="X49" s="3"/>
+      <c r="AA49" s="1"/>
+      <c r="AB49" s="3"/>
+      <c r="AC49" s="3"/>
+      <c r="AE49" s="1"/>
+      <c r="AF49" s="5"/>
+      <c r="AG49" s="5"/>
+    </row>
+    <row r="50" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="3"/>
+      <c r="AC50" s="3"/>
+      <c r="AE50" s="1"/>
+      <c r="AF50" s="5"/>
+      <c r="AG50" s="5"/>
+    </row>
+    <row r="51" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AA51" s="1"/>
+      <c r="AB51" s="3"/>
+      <c r="AC51" s="3"/>
+      <c r="AE51" s="1"/>
+      <c r="AF51" s="5"/>
+      <c r="AG51" s="5"/>
+    </row>
+    <row r="52" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AE52" s="1"/>
+      <c r="AF52" s="3"/>
+      <c r="AG52" s="3"/>
+    </row>
+    <row r="60" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AA60" s="1"/>
+      <c r="AB60" s="3"/>
+      <c r="AC60" s="3"/>
+      <c r="AE60" s="1"/>
+      <c r="AF60" s="5"/>
+      <c r="AG60" s="5"/>
+    </row>
+    <row r="61" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AA61" s="1"/>
+      <c r="AB61" s="3"/>
+      <c r="AC61" s="3"/>
+      <c r="AE61" s="1"/>
+      <c r="AF61" s="5"/>
+      <c r="AG61" s="5"/>
+    </row>
+    <row r="62" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AA62" s="1"/>
+      <c r="AB62" s="3"/>
+      <c r="AC62" s="3"/>
+      <c r="AE62" s="1"/>
+      <c r="AF62" s="5"/>
+      <c r="AG62" s="5"/>
+    </row>
+    <row r="63" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AA63" s="1"/>
+      <c r="AB63" s="3"/>
+      <c r="AC63" s="3"/>
+      <c r="AE63" s="1"/>
+      <c r="AF63" s="5"/>
+      <c r="AG63" s="5"/>
+    </row>
+    <row r="64" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AA64" s="1"/>
+      <c r="AB64" s="3"/>
+      <c r="AC64" s="3"/>
+      <c r="AE64" s="1"/>
+      <c r="AF64" s="5"/>
+      <c r="AG64" s="5"/>
+    </row>
+    <row r="65" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA65" s="1"/>
+      <c r="AB65" s="3"/>
+      <c r="AC65" s="3"/>
+      <c r="AE65" s="1"/>
+      <c r="AF65" s="5"/>
+      <c r="AG65" s="5"/>
+    </row>
+    <row r="66" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA66" s="1"/>
+      <c r="AB66" s="3"/>
+      <c r="AC66" s="3"/>
+      <c r="AE66" s="1"/>
+      <c r="AF66" s="5"/>
+      <c r="AG66" s="5"/>
+    </row>
+    <row r="67" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA67" s="1"/>
+      <c r="AB67" s="3"/>
+      <c r="AC67" s="3"/>
+      <c r="AE67" s="1"/>
+      <c r="AF67" s="5"/>
+      <c r="AG67" s="5"/>
+    </row>
+    <row r="68" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA68" s="1"/>
+      <c r="AB68" s="3"/>
+      <c r="AC68" s="3"/>
+      <c r="AE68" s="1"/>
+      <c r="AF68" s="5"/>
+      <c r="AG68" s="5"/>
+    </row>
+    <row r="69" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA69" s="1"/>
+      <c r="AB69" s="3"/>
+      <c r="AC69" s="3"/>
+      <c r="AE69" s="1"/>
+      <c r="AF69" s="5"/>
+      <c r="AG69" s="5"/>
+    </row>
+    <row r="70" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA70" s="1"/>
+      <c r="AB70" s="3"/>
+      <c r="AC70" s="3"/>
+      <c r="AE70" s="1"/>
+      <c r="AF70" s="5"/>
+      <c r="AG70" s="5"/>
+    </row>
+    <row r="71" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA71" s="1"/>
+      <c r="AB71" s="3"/>
+      <c r="AC71" s="3"/>
+      <c r="AE71" s="1"/>
+      <c r="AF71" s="5"/>
+      <c r="AG71" s="5"/>
+    </row>
+    <row r="72" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA72" s="1"/>
+      <c r="AB72" s="3"/>
+      <c r="AC72" s="3"/>
+      <c r="AE72" s="1"/>
+      <c r="AF72" s="5"/>
+      <c r="AG72" s="5"/>
+    </row>
+    <row r="73" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA73" s="1"/>
+      <c r="AB73" s="3"/>
+      <c r="AC73" s="3"/>
+      <c r="AE73" s="1"/>
+      <c r="AF73" s="5"/>
+      <c r="AG73" s="5"/>
+    </row>
+    <row r="74" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA74" s="1"/>
+      <c r="AB74" s="3"/>
+      <c r="AC74" s="3"/>
+      <c r="AE74" s="1"/>
+      <c r="AF74" s="5"/>
+      <c r="AG74" s="5"/>
+    </row>
+    <row r="75" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA75" s="1"/>
+      <c r="AB75" s="3"/>
+      <c r="AC75" s="3"/>
+      <c r="AE75" s="1"/>
+      <c r="AF75" s="5"/>
+      <c r="AG75" s="5"/>
+    </row>
+    <row r="76" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA76" s="1"/>
+      <c r="AB76" s="3"/>
+      <c r="AC76" s="3"/>
+      <c r="AE76" s="1"/>
+      <c r="AF76" s="5"/>
+      <c r="AG76" s="5"/>
+    </row>
+    <row r="77" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA77" s="1"/>
+      <c r="AB77" s="3"/>
+      <c r="AC77" s="3"/>
+      <c r="AE77" s="1"/>
+      <c r="AF77" s="5"/>
+      <c r="AG77" s="5"/>
+    </row>
+    <row r="78" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA78" s="1"/>
+      <c r="AB78" s="3"/>
+      <c r="AC78" s="3"/>
+      <c r="AE78" s="1"/>
+      <c r="AF78" s="5"/>
+      <c r="AG78" s="5"/>
+    </row>
+    <row r="79" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA79" s="1"/>
+      <c r="AB79" s="3"/>
+      <c r="AC79" s="3"/>
+      <c r="AE79" s="1"/>
+      <c r="AF79" s="5"/>
+      <c r="AG79" s="5"/>
+    </row>
+    <row r="80" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA80" s="1"/>
+      <c r="AB80" s="3"/>
+      <c r="AC80" s="3"/>
+      <c r="AE80" s="1"/>
+      <c r="AF80" s="5"/>
+      <c r="AG80" s="5"/>
+    </row>
+    <row r="81" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA81" s="1"/>
+      <c r="AB81" s="3"/>
+      <c r="AC81" s="3"/>
+      <c r="AE81" s="1"/>
+      <c r="AF81" s="5"/>
+      <c r="AG81" s="5"/>
+    </row>
+    <row r="82" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA82" s="1"/>
+      <c r="AB82" s="3"/>
+      <c r="AC82" s="3"/>
+      <c r="AE82" s="1"/>
+      <c r="AF82" s="5"/>
+      <c r="AG82" s="5"/>
+    </row>
+    <row r="83" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA83" s="1"/>
+      <c r="AB83" s="3"/>
+      <c r="AC83" s="3"/>
+      <c r="AE83" s="1"/>
+      <c r="AF83" s="5"/>
+      <c r="AG83" s="5"/>
+    </row>
+    <row r="84" spans="27:33" x14ac:dyDescent="0.25">
+      <c r="AA84" s="1"/>
+      <c r="AB84" s="3"/>
+      <c r="AC84" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="AB60:AD83">
-    <sortCondition ref="AB60"/>
+  <sortState ref="AE60:AG83">
+    <sortCondition ref="AE60"/>
   </sortState>
-  <mergeCells count="4">
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="N26:N31"/>
-    <mergeCell ref="P26:P31"/>
+  <mergeCells count="5">
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="R26:R31"/>
+    <mergeCell ref="S6:S11"/>
+    <mergeCell ref="N26:P31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Code version 27/06 16h
</commit_message>
<xml_diff>
--- a/Results_CG.xlsx
+++ b/Results_CG.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{157001E6-BFBC-4673-A483-48826F8FD31B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BC78FC36-FED7-42CD-9834-5C0F044C0C24}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="78">
   <si>
     <t>Instance name</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>Post-processing lv2 takes too much time (11m)</t>
+  </si>
+  <si>
+    <t>46h40min</t>
   </si>
 </sst>
 </file>
@@ -364,12 +367,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -656,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:AG84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
-      <selection activeCell="S50" sqref="S50"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,14 +697,14 @@
       </c>
     </row>
     <row r="4" spans="3:30" x14ac:dyDescent="0.25">
-      <c r="U4" s="15" t="s">
+      <c r="U4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15" t="s">
+      <c r="V4" s="17"/>
+      <c r="W4" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="X4" s="15"/>
+      <c r="X4" s="17"/>
       <c r="Z4" t="s">
         <v>38</v>
       </c>
@@ -809,7 +812,7 @@
       <c r="R6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="S6" s="15" t="s">
+      <c r="S6" s="17" t="s">
         <v>71</v>
       </c>
       <c r="T6" s="1"/>
@@ -878,7 +881,7 @@
       <c r="R7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="S7" s="15"/>
+      <c r="S7" s="17"/>
       <c r="T7" s="1"/>
       <c r="U7" s="3">
         <f t="shared" ref="U7:U10" si="0">(N7-I7)/I7</f>
@@ -948,7 +951,7 @@
       <c r="R8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="S8" s="15"/>
+      <c r="S8" s="17"/>
       <c r="T8" s="1"/>
       <c r="U8" s="3">
         <f t="shared" si="0"/>
@@ -1013,7 +1016,7 @@
         <v>45</v>
       </c>
       <c r="R9" s="7"/>
-      <c r="S9" s="15"/>
+      <c r="S9" s="17"/>
       <c r="T9" s="1"/>
       <c r="U9" s="3">
         <f t="shared" si="0"/>
@@ -1078,7 +1081,7 @@
         <v>45</v>
       </c>
       <c r="R10" s="7"/>
-      <c r="S10" s="15"/>
+      <c r="S10" s="17"/>
       <c r="T10" s="1"/>
       <c r="U10" s="3">
         <f t="shared" si="0"/>
@@ -1123,7 +1126,7 @@
         <v>45</v>
       </c>
       <c r="R11" s="7"/>
-      <c r="S11" s="15"/>
+      <c r="S11" s="17"/>
       <c r="T11" s="1"/>
       <c r="U11" s="3"/>
       <c r="V11" s="5"/>
@@ -1479,10 +1482,12 @@
       <c r="P20" s="14">
         <v>633</v>
       </c>
-      <c r="Q20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="R20" s="7"/>
+      <c r="Q20" s="4">
+        <v>644</v>
+      </c>
+      <c r="R20" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="S20" s="14"/>
       <c r="U20" s="3">
         <f t="shared" si="4"/>
@@ -1745,15 +1750,15 @@
       <c r="M26" s="2">
         <v>2415</v>
       </c>
-      <c r="N26" s="15" t="s">
+      <c r="N26" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
       <c r="Q26" s="2">
         <v>2415</v>
       </c>
-      <c r="R26" s="15" t="s">
+      <c r="R26" s="17" t="s">
         <v>66</v>
       </c>
       <c r="S26" s="14"/>
@@ -1807,13 +1812,13 @@
       <c r="M27" s="2">
         <v>2614</v>
       </c>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
       <c r="Q27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="R27" s="15"/>
+      <c r="R27" s="17"/>
       <c r="S27" s="14"/>
       <c r="U27" s="3">
         <f>(M27-I27)/I27</f>
@@ -1871,13 +1876,13 @@
       <c r="M28" s="2">
         <v>2660</v>
       </c>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
       <c r="Q28" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="R28" s="15"/>
+      <c r="R28" s="17"/>
       <c r="S28" s="14"/>
       <c r="U28" s="3">
         <f>(M28-I28)/I28</f>
@@ -1935,13 +1940,13 @@
       <c r="M29" s="2">
         <v>2734</v>
       </c>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
       <c r="Q29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="R29" s="15"/>
+      <c r="R29" s="17"/>
       <c r="S29" s="14"/>
       <c r="U29" s="3">
         <f>(M29-I29)/I29</f>
@@ -1999,13 +2004,13 @@
       <c r="M30" s="2">
         <v>2836</v>
       </c>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
       <c r="Q30" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="R30" s="15"/>
+      <c r="R30" s="17"/>
       <c r="S30" s="14"/>
       <c r="U30" s="3">
         <f>(M30-I30)/I30</f>
@@ -2052,13 +2057,13 @@
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
       <c r="Q31" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="R31" s="15"/>
+      <c r="R31" s="17"/>
       <c r="S31" s="14"/>
       <c r="U31" s="3"/>
       <c r="V31" s="5"/>
@@ -2591,7 +2596,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
       <c r="L41" s="11"/>
-      <c r="M41" s="16"/>
+      <c r="M41" s="15"/>
       <c r="Q41" s="4"/>
       <c r="R41" s="7"/>
       <c r="S41" s="14"/>
@@ -2781,7 +2786,7 @@
       <c r="M45" s="8">
         <v>15233</v>
       </c>
-      <c r="N45" s="17">
+      <c r="N45" s="16">
         <v>15274</v>
       </c>
       <c r="P45" s="14" t="s">
@@ -2852,7 +2857,7 @@
       <c r="M46" s="2">
         <v>15376</v>
       </c>
-      <c r="N46" s="17">
+      <c r="N46" s="16">
         <v>15765</v>
       </c>
       <c r="O46" s="14">
@@ -3020,7 +3025,7 @@
       <c r="O49" s="14">
         <v>16296</v>
       </c>
-      <c r="P49" s="17">
+      <c r="P49" s="16">
         <v>16415</v>
       </c>
       <c r="Q49" s="4" t="s">

</xml_diff>